<commit_message>
Updating esri maps with new shark data, adding more detailed legend labels
</commit_message>
<xml_diff>
--- a/tagging/data_raw/Argos_compiled.xlsx
+++ b/tagging/data_raw/Argos_compiled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/Github/emc/tagging/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6355E18B-E575-C048-A0A1-CB6B4DB83F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA7492-CCD4-0440-8AE6-2A0D3E5D5C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="283833PAT" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1392" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="182">
   <si>
     <t>PTTID</t>
   </si>
@@ -518,9 +518,6 @@
   </si>
   <si>
     <t>26354MINIPAT</t>
-  </si>
-  <si>
-    <t>2025-11-01</t>
   </si>
   <si>
     <t>2025-11-21</t>
@@ -579,10 +576,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="167" formatCode="0.0000000"/>
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -609,7 +606,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -632,16 +629,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -649,6 +658,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,7 +971,7 @@
   <dimension ref="A1:G256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1000,7 +1015,7 @@
       <c r="D3">
         <v>-61.879240000000003</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="9">
         <v>45832</v>
       </c>
     </row>
@@ -1017,7 +1032,7 @@
       <c r="D4">
         <v>-61.87941</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="9">
         <v>45838</v>
       </c>
     </row>
@@ -1034,7 +1049,7 @@
       <c r="D5">
         <v>-61.901040000000002</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="9">
         <v>45868</v>
       </c>
     </row>
@@ -1051,7 +1066,7 @@
       <c r="D6">
         <v>-61.921990000000001</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="9">
         <v>45873</v>
       </c>
     </row>
@@ -1068,7 +1083,7 @@
       <c r="D7">
         <v>-61.952629999999999</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="9">
         <v>45875</v>
       </c>
     </row>
@@ -1085,7 +1100,7 @@
       <c r="D8">
         <v>-61.997</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="9">
         <v>45894</v>
       </c>
     </row>
@@ -1102,7 +1117,7 @@
       <c r="D9">
         <v>-62.011270000000003</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="9">
         <v>45897</v>
       </c>
     </row>
@@ -1119,7 +1134,7 @@
       <c r="D10">
         <v>-61.99633</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="9">
         <v>45898</v>
       </c>
     </row>
@@ -1136,7 +1151,7 @@
       <c r="D11">
         <v>-61.956139999999998</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="9">
         <v>45909</v>
       </c>
     </row>
@@ -1153,7 +1168,7 @@
       <c r="D12">
         <v>-61.918379999999999</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="9">
         <v>45943</v>
       </c>
     </row>
@@ -6380,7 +6395,7 @@
   <dimension ref="A1:G271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6424,7 +6439,7 @@
       <c r="D3">
         <v>-61.951830000000001</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="9">
         <v>45840</v>
       </c>
     </row>
@@ -6441,7 +6456,7 @@
       <c r="D4">
         <v>-61.981389999999998</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="9">
         <v>45843</v>
       </c>
     </row>
@@ -6458,7 +6473,7 @@
       <c r="D5">
         <v>-61.936140000000002</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="9">
         <v>45849</v>
       </c>
     </row>
@@ -6475,7 +6490,7 @@
       <c r="D6">
         <v>-61.934190000000001</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="9">
         <v>45852</v>
       </c>
     </row>
@@ -6492,7 +6507,7 @@
       <c r="D7">
         <v>-61.950060000000001</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="9">
         <v>45857</v>
       </c>
     </row>
@@ -6509,7 +6524,7 @@
       <c r="D8">
         <v>-61.993160000000003</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="9">
         <v>45860</v>
       </c>
     </row>
@@ -6526,7 +6541,7 @@
       <c r="D9">
         <v>-62.02008</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="9">
         <v>45865</v>
       </c>
     </row>
@@ -6543,7 +6558,7 @@
       <c r="D10">
         <v>-62.025320000000001</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="9">
         <v>45870</v>
       </c>
     </row>
@@ -6560,7 +6575,7 @@
       <c r="D11">
         <v>-61.99371</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="9">
         <v>45873</v>
       </c>
     </row>
@@ -6577,7 +6592,7 @@
       <c r="D12">
         <v>-61.963799999999999</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="9">
         <v>45876</v>
       </c>
     </row>
@@ -6594,7 +6609,7 @@
       <c r="D13">
         <v>-61.983080000000001</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="9">
         <v>45883</v>
       </c>
     </row>
@@ -6611,7 +6626,7 @@
       <c r="D14">
         <v>-61.994579999999999</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="9">
         <v>45887</v>
       </c>
     </row>
@@ -6628,7 +6643,7 @@
       <c r="D15">
         <v>-61.947969999999998</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="9">
         <v>45890</v>
       </c>
     </row>
@@ -6645,7 +6660,7 @@
       <c r="D16">
         <v>-61.90954</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="9">
         <v>45894</v>
       </c>
     </row>
@@ -6662,7 +6677,7 @@
       <c r="D17">
         <v>-61.86092</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="9">
         <v>45897</v>
       </c>
     </row>
@@ -6679,7 +6694,7 @@
       <c r="D18">
         <v>-61.816589999999998</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="9">
         <v>45900</v>
       </c>
     </row>
@@ -6696,7 +6711,7 @@
       <c r="D19">
         <v>-61.779800000000002</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="9">
         <v>45909</v>
       </c>
     </row>
@@ -6713,7 +6728,7 @@
       <c r="D20">
         <v>-61.783790000000003</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="9">
         <v>45912</v>
       </c>
     </row>
@@ -6730,7 +6745,7 @@
       <c r="D21">
         <v>-61.789929999999998</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="9">
         <v>45915</v>
       </c>
     </row>
@@ -6747,7 +6762,7 @@
       <c r="D22">
         <v>-61.749960000000002</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="9">
         <v>45918</v>
       </c>
     </row>
@@ -6764,7 +6779,7 @@
       <c r="D23">
         <v>-61.779870000000003</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="9">
         <v>45921</v>
       </c>
     </row>
@@ -6781,7 +6796,7 @@
       <c r="D24">
         <v>-61.828029999999998</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="9">
         <v>45928</v>
       </c>
     </row>
@@ -6798,7 +6813,7 @@
       <c r="D25">
         <v>-61.809019999999997</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="9">
         <v>45931</v>
       </c>
     </row>
@@ -6815,7 +6830,7 @@
       <c r="D26">
         <v>-61.762390000000003</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="9">
         <v>45935</v>
       </c>
     </row>
@@ -6832,7 +6847,7 @@
       <c r="D27">
         <v>-61.758629999999997</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="9">
         <v>45940</v>
       </c>
     </row>
@@ -12056,10 +12071,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FEF50CA-A599-B44F-8ED0-C8714E499ECA}">
-  <dimension ref="A1:F136"/>
+  <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12073,37 +12088,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>16.759950799999999</v>
-      </c>
-      <c r="D2">
-        <v>-62.017498199999999</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -12111,16 +12114,16 @@
         <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>16.231853000000001</v>
+        <v>16.759950799999999</v>
       </c>
       <c r="D3">
-        <v>-62.683610399999999</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
+        <v>-62.017498199999999</v>
+      </c>
+      <c r="E3" s="11">
+        <v>45838</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -12128,16 +12131,16 @@
         <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>15.6539758</v>
+        <v>16.231853000000001</v>
       </c>
       <c r="D4">
-        <v>-63.516307300000001</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
+        <v>-62.683610399999999</v>
+      </c>
+      <c r="E4" s="11">
+        <v>45848</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -12145,16 +12148,16 @@
         <v>164</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>15.442717200000001</v>
+        <v>15.6539758</v>
       </c>
       <c r="D5">
-        <v>-63.269756999999998</v>
-      </c>
-      <c r="E5" t="s">
-        <v>90</v>
+        <v>-63.516307300000001</v>
+      </c>
+      <c r="E5" s="11">
+        <v>45863</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -12162,16 +12165,16 @@
         <v>164</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>14.714696999999999</v>
+        <v>15.442717200000001</v>
       </c>
       <c r="D6">
-        <v>-64.013177799999994</v>
-      </c>
-      <c r="E6" t="s">
-        <v>106</v>
+        <v>-63.269756999999998</v>
+      </c>
+      <c r="E6" s="11">
+        <v>45881</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -12179,16 +12182,16 @@
         <v>164</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>14.5744414</v>
+        <v>14.714696999999999</v>
       </c>
       <c r="D7">
-        <v>-63.350789300000002</v>
-      </c>
-      <c r="E7" t="s">
-        <v>124</v>
+        <v>-64.013177799999994</v>
+      </c>
+      <c r="E7" s="11">
+        <v>45897</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -12196,16 +12199,16 @@
         <v>164</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
-        <v>15.005031199999999</v>
+        <v>14.5744414</v>
       </c>
       <c r="D8">
-        <v>-61.813349799999997</v>
-      </c>
-      <c r="E8" t="s">
-        <v>142</v>
+        <v>-63.350789300000002</v>
+      </c>
+      <c r="E8" s="11">
+        <v>45915</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -12213,16 +12216,16 @@
         <v>164</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>16.033570399999999</v>
+        <v>15.005031199999999</v>
       </c>
       <c r="D9">
-        <v>-62.619306600000002</v>
-      </c>
-      <c r="E9" t="s">
-        <v>165</v>
+        <v>-61.813349799999997</v>
+      </c>
+      <c r="E9" s="11">
+        <v>45933</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -12230,56 +12233,58 @@
         <v>164</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>16.033570399999999</v>
+      </c>
+      <c r="D10">
+        <v>-62.619306600000002</v>
+      </c>
+      <c r="E10" s="11">
+        <v>45962</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>15.5275076</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>-63.427345099999997</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" s="11">
+        <v>45982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>30.1</v>
-      </c>
-      <c r="E13">
-        <v>28.9</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -12293,13 +12298,13 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>29.9</v>
+        <v>30.1</v>
       </c>
       <c r="E14">
-        <v>28.7</v>
+        <v>28.9</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -12313,13 +12318,13 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>29.6</v>
+        <v>29.9</v>
       </c>
       <c r="E15">
-        <v>28.4</v>
+        <v>28.7</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -12333,13 +12338,13 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>28.7</v>
+        <v>29.6</v>
       </c>
       <c r="E16">
-        <v>27.5</v>
+        <v>28.4</v>
       </c>
       <c r="F16">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -12347,19 +12352,19 @@
         <v>164</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>28.6</v>
+        <v>28.7</v>
       </c>
       <c r="E17">
-        <v>27.4</v>
+        <v>27.5</v>
       </c>
       <c r="F17">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -12373,13 +12378,13 @@
         <v>2</v>
       </c>
       <c r="D18">
-        <v>26.4</v>
+        <v>28.6</v>
       </c>
       <c r="E18">
-        <v>25.2</v>
+        <v>27.4</v>
       </c>
       <c r="F18">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -12387,19 +12392,19 @@
         <v>164</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>24.5</v>
+        <v>26.4</v>
       </c>
       <c r="E19">
-        <v>23.3</v>
+        <v>25.2</v>
       </c>
       <c r="F19">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -12413,13 +12418,13 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="E20">
-        <v>21.3</v>
+        <v>23.3</v>
       </c>
       <c r="F20">
-        <v>101</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -12427,19 +12432,19 @@
         <v>164</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>29.1</v>
+        <v>22.5</v>
       </c>
       <c r="E21">
-        <v>27.9</v>
+        <v>21.3</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -12453,13 +12458,13 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>27.6</v>
+        <v>29.1</v>
       </c>
       <c r="E22">
-        <v>26.4</v>
+        <v>27.9</v>
       </c>
       <c r="F22">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -12467,19 +12472,19 @@
         <v>164</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>25.9</v>
+        <v>27.6</v>
       </c>
       <c r="E23">
-        <v>24.7</v>
+        <v>26.4</v>
       </c>
       <c r="F23">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -12493,13 +12498,13 @@
         <v>5</v>
       </c>
       <c r="D24">
-        <v>23.2</v>
+        <v>25.9</v>
       </c>
       <c r="E24">
-        <v>22</v>
+        <v>24.7</v>
       </c>
       <c r="F24">
-        <v>89</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -12513,13 +12518,13 @@
         <v>5</v>
       </c>
       <c r="D25">
+        <v>23.2</v>
+      </c>
+      <c r="E25">
         <v>22</v>
       </c>
-      <c r="E25">
-        <v>20.8</v>
-      </c>
       <c r="F25">
-        <v>115</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -12527,19 +12532,19 @@
         <v>164</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>27.2</v>
+        <v>22</v>
       </c>
       <c r="E26">
-        <v>26</v>
+        <v>20.8</v>
       </c>
       <c r="F26">
-        <v>31</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -12547,19 +12552,19 @@
         <v>164</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27">
-        <v>28.1</v>
+        <v>27.2</v>
       </c>
       <c r="E27">
-        <v>26.9</v>
+        <v>26</v>
       </c>
       <c r="F27">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -12567,19 +12572,19 @@
         <v>164</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>24.2</v>
+        <v>28.1</v>
       </c>
       <c r="E28">
-        <v>23</v>
+        <v>26.9</v>
       </c>
       <c r="F28">
-        <v>74</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -12587,19 +12592,19 @@
         <v>164</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D29">
-        <v>20.6</v>
+        <v>24.2</v>
       </c>
       <c r="E29">
-        <v>19.399999999999999</v>
+        <v>23</v>
       </c>
       <c r="F29">
-        <v>142</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -12607,19 +12612,19 @@
         <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D30">
-        <v>28.8</v>
+        <v>20.6</v>
       </c>
       <c r="E30">
-        <v>27.6</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="F30">
-        <v>11</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -12627,19 +12632,19 @@
         <v>164</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>28.8</v>
+      </c>
+      <c r="E31">
+        <v>27.6</v>
+      </c>
+      <c r="F31">
         <v>11</v>
-      </c>
-      <c r="D31">
-        <v>24.8</v>
-      </c>
-      <c r="E31">
-        <v>23.6</v>
-      </c>
-      <c r="F31">
-        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -12647,19 +12652,19 @@
         <v>164</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>28.2</v>
+        <v>24.8</v>
       </c>
       <c r="E32">
-        <v>27</v>
+        <v>23.6</v>
       </c>
       <c r="F32">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -12667,19 +12672,19 @@
         <v>164</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>27.3</v>
+        <v>28.2</v>
       </c>
       <c r="E33">
-        <v>26.1</v>
+        <v>27</v>
       </c>
       <c r="F33">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -12693,13 +12698,13 @@
         <v>13</v>
       </c>
       <c r="D34">
-        <v>26</v>
+        <v>27.3</v>
       </c>
       <c r="E34">
-        <v>24.8</v>
+        <v>26.1</v>
       </c>
       <c r="F34">
-        <v>52</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -12707,19 +12712,19 @@
         <v>164</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E35">
-        <v>22.8</v>
+        <v>24.8</v>
       </c>
       <c r="F35">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -12733,13 +12738,13 @@
         <v>14</v>
       </c>
       <c r="D36">
-        <v>22.4</v>
+        <v>24</v>
       </c>
       <c r="E36">
-        <v>21.2</v>
+        <v>22.8</v>
       </c>
       <c r="F36">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -12747,19 +12752,19 @@
         <v>164</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37">
-        <v>20.3</v>
+        <v>22.4</v>
       </c>
       <c r="E37">
-        <v>19.100000000000001</v>
+        <v>21.2</v>
       </c>
       <c r="F37">
-        <v>141</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -12767,19 +12772,19 @@
         <v>164</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D38">
-        <v>28.3</v>
+        <v>20.3</v>
       </c>
       <c r="E38">
-        <v>27.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="F38">
-        <v>18</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -12787,19 +12792,19 @@
         <v>164</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D39">
-        <v>29.4</v>
+        <v>28.3</v>
       </c>
       <c r="E39">
-        <v>28.2</v>
+        <v>27.1</v>
       </c>
       <c r="F39">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -12807,19 +12812,19 @@
         <v>164</v>
       </c>
       <c r="B40" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C40">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40">
-        <v>22.1</v>
+        <v>29.4</v>
       </c>
       <c r="E40">
-        <v>20.9</v>
+        <v>28.2</v>
       </c>
       <c r="F40">
-        <v>111</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -12827,19 +12832,19 @@
         <v>164</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>26.5</v>
+        <v>22.1</v>
       </c>
       <c r="E41">
-        <v>25.3</v>
+        <v>20.9</v>
       </c>
       <c r="F41">
-        <v>45</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -12847,19 +12852,19 @@
         <v>164</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42">
-        <v>20.9</v>
+        <v>26.5</v>
       </c>
       <c r="E42">
-        <v>19.7</v>
+        <v>25.3</v>
       </c>
       <c r="F42">
-        <v>134</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -12867,19 +12872,19 @@
         <v>164</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C43">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D43">
-        <v>25.2</v>
+        <v>20.9</v>
       </c>
       <c r="E43">
-        <v>24</v>
+        <v>19.7</v>
       </c>
       <c r="F43">
-        <v>59</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -12887,19 +12892,19 @@
         <v>164</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44">
+        <v>23</v>
+      </c>
+      <c r="D44">
+        <v>25.2</v>
+      </c>
+      <c r="E44">
         <v>24</v>
       </c>
-      <c r="D44">
-        <v>22.9</v>
-      </c>
-      <c r="E44">
-        <v>21.7</v>
-      </c>
       <c r="F44">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -12907,19 +12912,19 @@
         <v>164</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45">
-        <v>29</v>
+        <v>22.9</v>
       </c>
       <c r="E45">
-        <v>27.8</v>
+        <v>21.7</v>
       </c>
       <c r="F45">
-        <v>11</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -12927,19 +12932,19 @@
         <v>164</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D46">
-        <v>24.6</v>
+        <v>29</v>
       </c>
       <c r="E46">
-        <v>23.4</v>
+        <v>27.8</v>
       </c>
       <c r="F46">
-        <v>67</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -12947,19 +12952,19 @@
         <v>164</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D47">
-        <v>28.4</v>
+        <v>24.6</v>
       </c>
       <c r="E47">
-        <v>27.2</v>
+        <v>23.4</v>
       </c>
       <c r="F47">
-        <v>14</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -12967,19 +12972,19 @@
         <v>164</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48">
+        <v>28.4</v>
+      </c>
+      <c r="E48">
         <v>27.2</v>
       </c>
-      <c r="E48">
-        <v>26</v>
-      </c>
       <c r="F48">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -12987,19 +12992,19 @@
         <v>164</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D49">
-        <v>25</v>
+        <v>27.2</v>
       </c>
       <c r="E49">
-        <v>23.8</v>
+        <v>26</v>
       </c>
       <c r="F49">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -13013,13 +13018,13 @@
         <v>29</v>
       </c>
       <c r="D50">
-        <v>22.6</v>
+        <v>25</v>
       </c>
       <c r="E50">
-        <v>21.4</v>
+        <v>23.8</v>
       </c>
       <c r="F50">
-        <v>103</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -13027,19 +13032,19 @@
         <v>164</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D51">
-        <v>20.2</v>
+        <v>22.6</v>
       </c>
       <c r="E51">
-        <v>19</v>
+        <v>21.4</v>
       </c>
       <c r="F51">
-        <v>143</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -13047,19 +13052,19 @@
         <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52">
-        <v>29.1</v>
+        <v>20.2</v>
       </c>
       <c r="E52">
-        <v>27.9</v>
+        <v>19</v>
       </c>
       <c r="F52">
-        <v>11</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -13067,19 +13072,19 @@
         <v>164</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D53">
-        <v>23.9</v>
+        <v>29.1</v>
       </c>
       <c r="E53">
-        <v>22.7</v>
+        <v>27.9</v>
       </c>
       <c r="F53">
-        <v>77</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -13087,19 +13092,19 @@
         <v>164</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D54">
-        <v>25.7</v>
+        <v>23.9</v>
       </c>
       <c r="E54">
-        <v>24.5</v>
+        <v>22.7</v>
       </c>
       <c r="F54">
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -13107,19 +13112,19 @@
         <v>164</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D55">
-        <v>23.2</v>
+        <v>25.7</v>
       </c>
       <c r="E55">
-        <v>22</v>
+        <v>24.5</v>
       </c>
       <c r="F55">
-        <v>91</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
@@ -13127,19 +13132,19 @@
         <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C56">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D56">
-        <v>21.3</v>
+        <v>23.2</v>
       </c>
       <c r="E56">
-        <v>20.100000000000001</v>
+        <v>22</v>
       </c>
       <c r="F56">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -13147,19 +13152,19 @@
         <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C57">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D57">
-        <v>28.2</v>
+        <v>21.3</v>
       </c>
       <c r="E57">
-        <v>27</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F57">
-        <v>18</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -13167,19 +13172,19 @@
         <v>164</v>
       </c>
       <c r="B58" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C58">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D58">
-        <v>29.5</v>
+        <v>28.2</v>
       </c>
       <c r="E58">
-        <v>28.3</v>
+        <v>27</v>
       </c>
       <c r="F58">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -13187,19 +13192,19 @@
         <v>164</v>
       </c>
       <c r="B59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C59">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D59">
-        <v>21</v>
+        <v>29.5</v>
       </c>
       <c r="E59">
-        <v>19.8</v>
+        <v>28.3</v>
       </c>
       <c r="F59">
-        <v>134</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -13207,19 +13212,19 @@
         <v>164</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C60">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D60">
-        <v>26.7</v>
+        <v>21</v>
       </c>
       <c r="E60">
-        <v>25.5</v>
+        <v>19.8</v>
       </c>
       <c r="F60">
-        <v>43</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -13227,19 +13232,19 @@
         <v>164</v>
       </c>
       <c r="B61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C61">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D61">
-        <v>25.1</v>
+        <v>26.7</v>
       </c>
       <c r="E61">
-        <v>23.9</v>
+        <v>25.5</v>
       </c>
       <c r="F61">
-        <v>63</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
@@ -13247,19 +13252,19 @@
         <v>164</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C62">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D62">
-        <v>28</v>
+        <v>25.1</v>
       </c>
       <c r="E62">
-        <v>26.8</v>
+        <v>23.9</v>
       </c>
       <c r="F62">
-        <v>19</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
@@ -13267,19 +13272,19 @@
         <v>164</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C63">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D63">
-        <v>26.6</v>
+        <v>28</v>
       </c>
       <c r="E63">
-        <v>25.4</v>
+        <v>26.8</v>
       </c>
       <c r="F63">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -13287,19 +13292,19 @@
         <v>164</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C64">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D64">
-        <v>24.3</v>
+        <v>26.6</v>
       </c>
       <c r="E64">
-        <v>23.1</v>
+        <v>25.4</v>
       </c>
       <c r="F64">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -13313,13 +13318,13 @@
         <v>47</v>
       </c>
       <c r="D65">
-        <v>22.4</v>
+        <v>24.3</v>
       </c>
       <c r="E65">
-        <v>21.2</v>
+        <v>23.1</v>
       </c>
       <c r="F65">
-        <v>101</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -13327,19 +13332,19 @@
         <v>164</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C66">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D66">
-        <v>20</v>
+        <v>22.4</v>
       </c>
       <c r="E66">
-        <v>18.8</v>
+        <v>21.2</v>
       </c>
       <c r="F66">
-        <v>144</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -13347,19 +13352,19 @@
         <v>164</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C67">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D67">
-        <v>29.2</v>
+        <v>20</v>
       </c>
       <c r="E67">
-        <v>28</v>
+        <v>18.8</v>
       </c>
       <c r="F67">
-        <v>8</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -13367,19 +13372,19 @@
         <v>164</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C68">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D68">
-        <v>25.2</v>
+        <v>29.2</v>
       </c>
       <c r="E68">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F68">
-        <v>58</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -13387,19 +13392,19 @@
         <v>164</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C69">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D69">
-        <v>20.8</v>
+        <v>25.2</v>
       </c>
       <c r="E69">
-        <v>19.600000000000001</v>
+        <v>24</v>
       </c>
       <c r="F69">
-        <v>132</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -13407,19 +13412,19 @@
         <v>164</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C70">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D70">
-        <v>23.1</v>
+        <v>20.8</v>
       </c>
       <c r="E70">
-        <v>21.9</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F70">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -13427,19 +13432,19 @@
         <v>164</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C71">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D71">
-        <v>28.9</v>
+        <v>23.1</v>
       </c>
       <c r="E71">
-        <v>27.7</v>
+        <v>21.9</v>
       </c>
       <c r="F71">
-        <v>11</v>
+        <v>97</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -13447,19 +13452,19 @@
         <v>164</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C72">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D72">
-        <v>26.7</v>
+        <v>28.9</v>
       </c>
       <c r="E72">
-        <v>25.5</v>
+        <v>27.7</v>
       </c>
       <c r="F72">
-        <v>43</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -13467,19 +13472,19 @@
         <v>164</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C73">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D73">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="E73">
-        <v>23.5</v>
+        <v>25.5</v>
       </c>
       <c r="F73">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -13487,19 +13492,19 @@
         <v>164</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C74">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D74">
-        <v>22</v>
+        <v>24.7</v>
       </c>
       <c r="E74">
-        <v>20.8</v>
+        <v>23.5</v>
       </c>
       <c r="F74">
-        <v>112</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -13507,19 +13512,19 @@
         <v>164</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C75">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D75">
-        <v>27.5</v>
+        <v>22</v>
       </c>
       <c r="E75">
-        <v>26.3</v>
+        <v>20.8</v>
       </c>
       <c r="F75">
-        <v>27</v>
+        <v>112</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -13527,19 +13532,19 @@
         <v>164</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C76">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D76">
-        <v>29.6</v>
+        <v>27.5</v>
       </c>
       <c r="E76">
-        <v>28.4</v>
+        <v>26.3</v>
       </c>
       <c r="F76">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -13547,19 +13552,19 @@
         <v>164</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C77">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D77">
-        <v>27.9</v>
+        <v>29.6</v>
       </c>
       <c r="E77">
-        <v>26.7</v>
+        <v>28.4</v>
       </c>
       <c r="F77">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -13567,19 +13572,19 @@
         <v>164</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C78">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D78">
-        <v>25.9</v>
+        <v>27.9</v>
       </c>
       <c r="E78">
-        <v>24.7</v>
+        <v>26.7</v>
       </c>
       <c r="F78">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -13587,19 +13592,19 @@
         <v>164</v>
       </c>
       <c r="B79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C79">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D79">
-        <v>24.2</v>
+        <v>25.9</v>
       </c>
       <c r="E79">
-        <v>23</v>
+        <v>24.7</v>
       </c>
       <c r="F79">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
@@ -13607,19 +13612,19 @@
         <v>164</v>
       </c>
       <c r="B80" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C80">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D80">
-        <v>21.6</v>
+        <v>24.2</v>
       </c>
       <c r="E80">
-        <v>20.399999999999999</v>
+        <v>23</v>
       </c>
       <c r="F80">
-        <v>118</v>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -13627,19 +13632,19 @@
         <v>164</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C81">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D81">
-        <v>20.9</v>
+        <v>21.6</v>
       </c>
       <c r="E81">
-        <v>19.7</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="F81">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -13647,19 +13652,19 @@
         <v>164</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C82">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D82">
-        <v>28.1</v>
+        <v>20.9</v>
       </c>
       <c r="E82">
-        <v>26.9</v>
+        <v>19.7</v>
       </c>
       <c r="F82">
-        <v>16</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -13667,19 +13672,19 @@
         <v>164</v>
       </c>
       <c r="B83" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C83">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D83">
-        <v>26.6</v>
+        <v>28.1</v>
       </c>
       <c r="E83">
-        <v>25.4</v>
+        <v>26.9</v>
       </c>
       <c r="F83">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -13687,19 +13692,19 @@
         <v>164</v>
       </c>
       <c r="B84" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C84">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D84">
-        <v>19.600000000000001</v>
+        <v>26.6</v>
       </c>
       <c r="E84">
-        <v>18.399999999999999</v>
+        <v>25.4</v>
       </c>
       <c r="F84">
-        <v>154</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -13707,19 +13712,19 @@
         <v>164</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C85">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D85">
-        <v>23.3</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E85">
-        <v>22.1</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="F85">
-        <v>96</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -13727,19 +13732,19 @@
         <v>164</v>
       </c>
       <c r="B86" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C86">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D86">
-        <v>24.4</v>
+        <v>23.3</v>
       </c>
       <c r="E86">
-        <v>23.2</v>
+        <v>22.1</v>
       </c>
       <c r="F86">
-        <v>77</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -13747,19 +13752,19 @@
         <v>164</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C87">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D87">
-        <v>25.9</v>
+        <v>24.4</v>
       </c>
       <c r="E87">
-        <v>24.7</v>
+        <v>23.2</v>
       </c>
       <c r="F87">
-        <v>54</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -13767,19 +13772,19 @@
         <v>164</v>
       </c>
       <c r="B88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C88">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D88">
-        <v>27.4</v>
+        <v>25.9</v>
       </c>
       <c r="E88">
-        <v>26.2</v>
+        <v>24.7</v>
       </c>
       <c r="F88">
-        <v>29</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
@@ -13787,19 +13792,19 @@
         <v>164</v>
       </c>
       <c r="B89" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C89">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D89">
-        <v>28.7</v>
+        <v>27.4</v>
       </c>
       <c r="E89">
-        <v>27.5</v>
+        <v>26.2</v>
       </c>
       <c r="F89">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -13807,19 +13812,19 @@
         <v>164</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C90">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D90">
-        <v>20.100000000000001</v>
+        <v>28.7</v>
       </c>
       <c r="E90">
-        <v>18.899999999999999</v>
+        <v>27.5</v>
       </c>
       <c r="F90">
-        <v>144</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
@@ -13827,19 +13832,19 @@
         <v>164</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C91">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D91">
-        <v>27.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="E91">
-        <v>25.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="F91">
-        <v>33</v>
+        <v>144</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -13847,19 +13852,19 @@
         <v>164</v>
       </c>
       <c r="B92" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C92">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D92">
-        <v>28.5</v>
+        <v>27.1</v>
       </c>
       <c r="E92">
-        <v>27.3</v>
+        <v>25.9</v>
       </c>
       <c r="F92">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -13873,13 +13878,13 @@
         <v>89</v>
       </c>
       <c r="D93">
-        <v>27.2</v>
+        <v>28.5</v>
       </c>
       <c r="E93">
-        <v>26</v>
+        <v>27.3</v>
       </c>
       <c r="F93">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
@@ -13887,19 +13892,19 @@
         <v>164</v>
       </c>
       <c r="B94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C94">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D94">
-        <v>24.4</v>
+        <v>27.2</v>
       </c>
       <c r="E94">
-        <v>23.2</v>
+        <v>26</v>
       </c>
       <c r="F94">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
@@ -13913,13 +13918,13 @@
         <v>90</v>
       </c>
       <c r="D95">
-        <v>22.3</v>
+        <v>24.4</v>
       </c>
       <c r="E95">
-        <v>21.1</v>
+        <v>23.2</v>
       </c>
       <c r="F95">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -13927,19 +13932,19 @@
         <v>164</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C96">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D96">
-        <v>19.8</v>
+        <v>22.3</v>
       </c>
       <c r="E96">
-        <v>18.600000000000001</v>
+        <v>21.1</v>
       </c>
       <c r="F96">
-        <v>147</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -13947,19 +13952,19 @@
         <v>164</v>
       </c>
       <c r="B97" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C97">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D97">
-        <v>29.2</v>
+        <v>19.8</v>
       </c>
       <c r="E97">
-        <v>28</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="F97">
-        <v>9</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -13967,19 +13972,19 @@
         <v>164</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C98">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D98">
-        <v>25.7</v>
+        <v>29.2</v>
       </c>
       <c r="E98">
-        <v>24.5</v>
+        <v>28</v>
       </c>
       <c r="F98">
-        <v>55</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -13987,19 +13992,19 @@
         <v>164</v>
       </c>
       <c r="B99" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C99">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D99">
-        <v>23.5</v>
+        <v>25.7</v>
       </c>
       <c r="E99">
-        <v>22.3</v>
+        <v>24.5</v>
       </c>
       <c r="F99">
-        <v>89</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -14007,19 +14012,19 @@
         <v>164</v>
       </c>
       <c r="B100" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C100">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D100">
-        <v>21.3</v>
+        <v>23.5</v>
       </c>
       <c r="E100">
-        <v>20.100000000000001</v>
+        <v>22.3</v>
       </c>
       <c r="F100">
-        <v>121</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -14027,19 +14032,19 @@
         <v>164</v>
       </c>
       <c r="B101" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C101">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D101">
-        <v>28.2</v>
+        <v>21.3</v>
       </c>
       <c r="E101">
-        <v>27</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F101">
-        <v>17</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -14047,19 +14052,19 @@
         <v>164</v>
       </c>
       <c r="B102" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C102">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D102">
-        <v>26.8</v>
+        <v>28.2</v>
       </c>
       <c r="E102">
-        <v>25.6</v>
+        <v>27</v>
       </c>
       <c r="F102">
-        <v>39</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -14067,19 +14072,19 @@
         <v>164</v>
       </c>
       <c r="B103" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C103">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D103">
-        <v>24.2</v>
+        <v>26.8</v>
       </c>
       <c r="E103">
-        <v>23</v>
+        <v>25.6</v>
       </c>
       <c r="F103">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
@@ -14087,19 +14092,19 @@
         <v>164</v>
       </c>
       <c r="B104" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C104">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D104">
-        <v>29.1</v>
+        <v>24.2</v>
       </c>
       <c r="E104">
-        <v>27.9</v>
+        <v>23</v>
       </c>
       <c r="F104">
-        <v>11</v>
+        <v>72</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -14113,13 +14118,13 @@
         <v>102</v>
       </c>
       <c r="D105">
-        <v>20.5</v>
+        <v>29.1</v>
       </c>
       <c r="E105">
-        <v>19.3</v>
+        <v>27.9</v>
       </c>
       <c r="F105">
-        <v>140</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -14127,19 +14132,19 @@
         <v>164</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C106">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D106">
-        <v>24.9</v>
+        <v>20.5</v>
       </c>
       <c r="E106">
-        <v>23.7</v>
+        <v>19.3</v>
       </c>
       <c r="F106">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
@@ -14147,19 +14152,19 @@
         <v>164</v>
       </c>
       <c r="B107" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C107">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D107">
-        <v>28.1</v>
+        <v>24.9</v>
       </c>
       <c r="E107">
-        <v>26.9</v>
+        <v>23.7</v>
       </c>
       <c r="F107">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
@@ -14167,19 +14172,19 @@
         <v>164</v>
       </c>
       <c r="B108" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C108">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D108">
-        <v>26.2</v>
+        <v>28.1</v>
       </c>
       <c r="E108">
-        <v>25</v>
+        <v>26.9</v>
       </c>
       <c r="F108">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -14187,19 +14192,19 @@
         <v>164</v>
       </c>
       <c r="B109" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C109">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D109">
-        <v>24.2</v>
+        <v>26.2</v>
       </c>
       <c r="E109">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F109">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -14207,19 +14212,19 @@
         <v>164</v>
       </c>
       <c r="B110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C110">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D110">
-        <v>22.1</v>
+        <v>24.2</v>
       </c>
       <c r="E110">
-        <v>20.9</v>
+        <v>23</v>
       </c>
       <c r="F110">
-        <v>113</v>
+        <v>76</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -14227,19 +14232,19 @@
         <v>164</v>
       </c>
       <c r="B111" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C111">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D111">
-        <v>19.5</v>
+        <v>22.1</v>
       </c>
       <c r="E111">
-        <v>18.3</v>
+        <v>20.9</v>
       </c>
       <c r="F111">
-        <v>156</v>
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -14247,19 +14252,19 @@
         <v>164</v>
       </c>
       <c r="B112" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C112">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D112">
-        <v>29</v>
+        <v>19.5</v>
       </c>
       <c r="E112">
-        <v>27.8</v>
+        <v>18.3</v>
       </c>
       <c r="F112">
-        <v>9</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
@@ -14267,19 +14272,19 @@
         <v>164</v>
       </c>
       <c r="B113" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C113">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D113">
-        <v>25.7</v>
+        <v>29</v>
       </c>
       <c r="E113">
-        <v>24.5</v>
+        <v>27.8</v>
       </c>
       <c r="F113">
-        <v>54</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -14287,19 +14292,19 @@
         <v>164</v>
       </c>
       <c r="B114" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C114">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D114">
-        <v>23.4</v>
+        <v>25.7</v>
       </c>
       <c r="E114">
-        <v>22.2</v>
+        <v>24.5</v>
       </c>
       <c r="F114">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -14307,19 +14312,19 @@
         <v>164</v>
       </c>
       <c r="B115" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C115">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D115">
-        <v>20.399999999999999</v>
+        <v>23.4</v>
       </c>
       <c r="E115">
-        <v>19.2</v>
+        <v>22.2</v>
       </c>
       <c r="F115">
-        <v>142</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
@@ -14327,19 +14332,19 @@
         <v>164</v>
       </c>
       <c r="B116" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C116">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D116">
-        <v>21.6</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="E116">
-        <v>20.399999999999999</v>
+        <v>19.2</v>
       </c>
       <c r="F116">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -14347,19 +14352,19 @@
         <v>164</v>
       </c>
       <c r="B117" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C117">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D117">
-        <v>24.5</v>
+        <v>21.6</v>
       </c>
       <c r="E117">
-        <v>23.3</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="F117">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
@@ -14367,19 +14372,19 @@
         <v>164</v>
       </c>
       <c r="B118" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C118">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D118">
-        <v>26.9</v>
+        <v>24.5</v>
       </c>
       <c r="E118">
-        <v>25.7</v>
+        <v>23.3</v>
       </c>
       <c r="F118">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
@@ -14387,19 +14392,19 @@
         <v>164</v>
       </c>
       <c r="B119" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C119">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D119">
-        <v>28.4</v>
+        <v>26.9</v>
       </c>
       <c r="E119">
-        <v>27.2</v>
+        <v>25.7</v>
       </c>
       <c r="F119">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -14407,19 +14412,19 @@
         <v>164</v>
       </c>
       <c r="B120" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C120">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D120">
-        <v>29.3</v>
+        <v>28.4</v>
       </c>
       <c r="E120">
-        <v>28.1</v>
+        <v>27.2</v>
       </c>
       <c r="F120">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -14427,19 +14432,19 @@
         <v>164</v>
       </c>
       <c r="B121" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C121">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D121">
-        <v>29.7</v>
+        <v>29.3</v>
       </c>
       <c r="E121">
-        <v>28.5</v>
+        <v>28.1</v>
       </c>
       <c r="F121">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -14447,19 +14452,19 @@
         <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C122">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D122">
-        <v>27.9</v>
+        <v>29.7</v>
       </c>
       <c r="E122">
-        <v>26.7</v>
+        <v>28.5</v>
       </c>
       <c r="F122">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -14467,19 +14472,19 @@
         <v>164</v>
       </c>
       <c r="B123" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C123">
         <v>143</v>
       </c>
       <c r="D123">
-        <v>26.6</v>
+        <v>27.9</v>
       </c>
       <c r="E123">
-        <v>25.4</v>
+        <v>26.7</v>
       </c>
       <c r="F123">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -14487,19 +14492,19 @@
         <v>164</v>
       </c>
       <c r="B124" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C124">
         <v>143</v>
       </c>
       <c r="D124">
-        <v>24.5</v>
+        <v>26.6</v>
       </c>
       <c r="E124">
-        <v>23.3</v>
+        <v>25.4</v>
       </c>
       <c r="F124">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -14507,19 +14512,19 @@
         <v>164</v>
       </c>
       <c r="B125" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C125">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D125">
-        <v>28.8</v>
+        <v>24.5</v>
       </c>
       <c r="E125">
-        <v>27.6</v>
+        <v>23.3</v>
       </c>
       <c r="F125">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -14527,19 +14532,19 @@
         <v>164</v>
       </c>
       <c r="B126" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C126">
         <v>144</v>
       </c>
       <c r="D126">
-        <v>25.8</v>
+        <v>28.8</v>
       </c>
       <c r="E126">
-        <v>24.6</v>
+        <v>27.6</v>
       </c>
       <c r="F126">
-        <v>55</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -14547,19 +14552,19 @@
         <v>164</v>
       </c>
       <c r="B127" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C127">
         <v>144</v>
       </c>
       <c r="D127">
-        <v>23.1</v>
+        <v>25.8</v>
       </c>
       <c r="E127">
-        <v>21.9</v>
+        <v>24.6</v>
       </c>
       <c r="F127">
-        <v>93</v>
+        <v>55</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -14567,19 +14572,19 @@
         <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C128">
         <v>144</v>
       </c>
       <c r="D128">
-        <v>21.8</v>
+        <v>23.1</v>
       </c>
       <c r="E128">
-        <v>20.6</v>
+        <v>21.9</v>
       </c>
       <c r="F128">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -14587,19 +14592,19 @@
         <v>164</v>
       </c>
       <c r="B129" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C129">
         <v>144</v>
       </c>
       <c r="D129">
-        <v>19.100000000000001</v>
+        <v>21.8</v>
       </c>
       <c r="E129">
-        <v>17.899999999999999</v>
+        <v>20.6</v>
       </c>
       <c r="F129">
-        <v>164</v>
+        <v>118</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -14607,19 +14612,19 @@
         <v>164</v>
       </c>
       <c r="B130" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C130">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D130">
-        <v>30.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E130">
-        <v>28.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="F130">
-        <v>1</v>
+        <v>164</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -14627,19 +14632,19 @@
         <v>164</v>
       </c>
       <c r="B131" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C131">
         <v>145</v>
       </c>
       <c r="D131">
-        <v>30</v>
+        <v>30.1</v>
       </c>
       <c r="E131">
-        <v>28.8</v>
+        <v>28.9</v>
       </c>
       <c r="F131">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -14647,7 +14652,7 @@
         <v>164</v>
       </c>
       <c r="B132" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C132">
         <v>145</v>
@@ -14667,19 +14672,19 @@
         <v>164</v>
       </c>
       <c r="B133" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C133">
         <v>145</v>
       </c>
       <c r="D133">
-        <v>29.9</v>
+        <v>30</v>
       </c>
       <c r="E133">
-        <v>28.7</v>
+        <v>28.8</v>
       </c>
       <c r="F133">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -14687,19 +14692,19 @@
         <v>164</v>
       </c>
       <c r="B134" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C134">
         <v>145</v>
       </c>
       <c r="D134">
-        <v>29.8</v>
+        <v>29.9</v>
       </c>
       <c r="E134">
-        <v>28.6</v>
+        <v>28.7</v>
       </c>
       <c r="F134">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -14707,19 +14712,19 @@
         <v>164</v>
       </c>
       <c r="B135" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C135">
         <v>145</v>
       </c>
       <c r="D135">
-        <v>29.6</v>
+        <v>29.8</v>
       </c>
       <c r="E135">
-        <v>28.4</v>
+        <v>28.6</v>
       </c>
       <c r="F135">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -14727,18 +14732,38 @@
         <v>164</v>
       </c>
       <c r="B136" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C136">
         <v>145</v>
       </c>
       <c r="D136">
+        <v>29.6</v>
+      </c>
+      <c r="E136">
+        <v>28.4</v>
+      </c>
+      <c r="F136">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>164</v>
+      </c>
+      <c r="B137" t="s">
+        <v>165</v>
+      </c>
+      <c r="C137">
+        <v>145</v>
+      </c>
+      <c r="D137">
         <v>29.4</v>
       </c>
-      <c r="E136">
+      <c r="E137">
         <v>28.2</v>
       </c>
-      <c r="F136">
+      <c r="F137">
         <v>7</v>
       </c>
     </row>
@@ -14749,10 +14774,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2803F26B-B814-704C-B2A0-A5DB14B7449B}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14763,400 +14788,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>16.722611000000001</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>-62.551471499999998</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="10">
         <v>45838</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>16.907081399999999</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>-62.973188200000003</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="10">
         <v>45884</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>16.6669147</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>-63.201355999999997</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="10">
         <v>45982</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>162</v>
+      <c r="A7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>60</v>
+      <c r="A8" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45838</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>28.88</v>
+      </c>
+      <c r="E8" s="3">
+        <v>27.52</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6.6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9" s="6">
-        <v>45838</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>28.88</v>
-      </c>
-      <c r="E9" s="4">
-        <v>27.52</v>
-      </c>
-      <c r="F9" s="3">
-        <v>6.6</v>
+      <c r="A9" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="5">
+        <v>45843</v>
+      </c>
+      <c r="C9" s="4">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3">
+        <v>27.37</v>
+      </c>
+      <c r="E9" s="3">
+        <v>26.09</v>
+      </c>
+      <c r="F9" s="2">
+        <v>30.6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45843</v>
-      </c>
-      <c r="C10" s="5">
-        <v>6</v>
-      </c>
-      <c r="D10" s="4">
-        <v>27.37</v>
-      </c>
-      <c r="E10" s="4">
-        <v>26.09</v>
-      </c>
-      <c r="F10" s="3">
-        <v>30.6</v>
+      <c r="A10" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="5">
+        <v>45848</v>
+      </c>
+      <c r="C10" s="4">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3">
+        <v>22.27</v>
+      </c>
+      <c r="E10" s="3">
+        <v>20.92</v>
+      </c>
+      <c r="F10" s="2">
+        <v>172.8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B11" s="6">
-        <v>45848</v>
-      </c>
-      <c r="C11" s="5">
-        <v>11</v>
-      </c>
-      <c r="D11" s="4">
-        <v>22.27</v>
-      </c>
-      <c r="E11" s="4">
-        <v>20.92</v>
-      </c>
-      <c r="F11" s="3">
-        <v>172.8</v>
+      <c r="A11" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="5">
+        <v>45853</v>
+      </c>
+      <c r="C11" s="4">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>22.84</v>
+      </c>
+      <c r="E11" s="3">
+        <v>21.45</v>
+      </c>
+      <c r="F11" s="2">
+        <v>117.2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="6">
-        <v>45853</v>
-      </c>
-      <c r="C12" s="5">
-        <v>16</v>
-      </c>
-      <c r="D12" s="4">
-        <v>22.84</v>
-      </c>
-      <c r="E12" s="4">
-        <v>21.45</v>
-      </c>
-      <c r="F12" s="3">
-        <v>117.2</v>
+      <c r="A12" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45860</v>
+      </c>
+      <c r="C12" s="4">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3">
+        <v>22.73</v>
+      </c>
+      <c r="E12" s="3">
+        <v>21.46</v>
+      </c>
+      <c r="F12" s="2">
+        <v>147.19999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" s="6">
-        <v>45860</v>
-      </c>
-      <c r="C13" s="5">
-        <v>23</v>
-      </c>
-      <c r="D13" s="4">
-        <v>22.73</v>
-      </c>
-      <c r="E13" s="4">
-        <v>21.46</v>
-      </c>
-      <c r="F13" s="3">
-        <v>147.19999999999999</v>
+      <c r="A13" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="5">
+        <v>45868</v>
+      </c>
+      <c r="C13" s="4">
+        <v>31</v>
+      </c>
+      <c r="D13" s="3">
+        <v>22.97</v>
+      </c>
+      <c r="E13" s="3">
+        <v>21.74</v>
+      </c>
+      <c r="F13" s="2">
+        <v>126.2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" s="6">
-        <v>45868</v>
-      </c>
-      <c r="C14" s="5">
-        <v>31</v>
-      </c>
-      <c r="D14" s="4">
-        <v>22.97</v>
-      </c>
-      <c r="E14" s="4">
-        <v>21.74</v>
-      </c>
-      <c r="F14" s="3">
-        <v>126.2</v>
+      <c r="A14" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="5">
+        <v>45884</v>
+      </c>
+      <c r="C14" s="4">
+        <v>47</v>
+      </c>
+      <c r="D14" s="3">
+        <v>22.82</v>
+      </c>
+      <c r="E14" s="3">
+        <v>21.53</v>
+      </c>
+      <c r="F14" s="2">
+        <v>119.9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15" s="6">
-        <v>45884</v>
-      </c>
-      <c r="C15" s="5">
-        <v>47</v>
-      </c>
-      <c r="D15" s="4">
-        <v>22.82</v>
-      </c>
-      <c r="E15" s="4">
-        <v>21.53</v>
-      </c>
-      <c r="F15" s="3">
-        <v>119.9</v>
+      <c r="A15" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="5">
+        <v>45896</v>
+      </c>
+      <c r="C15" s="4">
+        <v>59</v>
+      </c>
+      <c r="D15" s="3">
+        <v>21.58</v>
+      </c>
+      <c r="E15" s="3">
+        <v>20.21</v>
+      </c>
+      <c r="F15" s="2">
+        <v>155.9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B16" s="6">
-        <v>45896</v>
-      </c>
-      <c r="C16" s="5">
-        <v>59</v>
-      </c>
-      <c r="D16" s="4">
-        <v>21.58</v>
-      </c>
-      <c r="E16" s="4">
-        <v>20.21</v>
-      </c>
-      <c r="F16" s="3">
-        <v>155.9</v>
+      <c r="A16" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="5">
+        <v>45909</v>
+      </c>
+      <c r="C16" s="4">
+        <v>72</v>
+      </c>
+      <c r="D16" s="3">
+        <v>21.36</v>
+      </c>
+      <c r="E16" s="3">
+        <v>20.04</v>
+      </c>
+      <c r="F16" s="2">
+        <v>150.5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B17" s="6">
-        <v>45909</v>
-      </c>
-      <c r="C17" s="5">
-        <v>72</v>
-      </c>
-      <c r="D17" s="4">
-        <v>21.36</v>
-      </c>
-      <c r="E17" s="4">
-        <v>20.04</v>
-      </c>
-      <c r="F17" s="3">
-        <v>150.5</v>
+      <c r="A17" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="5">
+        <v>45924</v>
+      </c>
+      <c r="C17" s="4">
+        <v>87</v>
+      </c>
+      <c r="D17" s="3">
+        <v>27.36</v>
+      </c>
+      <c r="E17" s="3">
+        <v>26.25</v>
+      </c>
+      <c r="F17" s="2">
+        <v>32.5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B18" s="6">
-        <v>45924</v>
-      </c>
-      <c r="C18" s="5">
-        <v>87</v>
-      </c>
-      <c r="D18" s="4">
-        <v>27.36</v>
-      </c>
-      <c r="E18" s="4">
-        <v>26.25</v>
-      </c>
-      <c r="F18" s="3">
-        <v>32.5</v>
+      <c r="A18" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="5">
+        <v>45939</v>
+      </c>
+      <c r="C18" s="4">
+        <v>102</v>
+      </c>
+      <c r="D18" s="3">
+        <v>21.65</v>
+      </c>
+      <c r="E18" s="3">
+        <v>20.48</v>
+      </c>
+      <c r="F18" s="2">
+        <v>100.8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B19" s="6">
-        <v>45939</v>
-      </c>
-      <c r="C19" s="5">
-        <v>102</v>
-      </c>
-      <c r="D19" s="4">
-        <v>21.65</v>
-      </c>
-      <c r="E19" s="4">
-        <v>20.48</v>
-      </c>
-      <c r="F19" s="3">
-        <v>100.8</v>
+      <c r="A19" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="5">
+        <v>45954</v>
+      </c>
+      <c r="C19" s="4">
+        <v>117</v>
+      </c>
+      <c r="D19" s="3">
+        <v>23.02</v>
+      </c>
+      <c r="E19" s="3">
+        <v>21.77</v>
+      </c>
+      <c r="F19" s="2">
+        <v>145.69999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" s="6">
-        <v>45954</v>
-      </c>
-      <c r="C20" s="5">
-        <v>117</v>
-      </c>
-      <c r="D20" s="4">
-        <v>23.02</v>
-      </c>
-      <c r="E20" s="4">
-        <v>21.77</v>
-      </c>
-      <c r="F20" s="3">
-        <v>145.69999999999999</v>
+      <c r="A20" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="5">
+        <v>45969</v>
+      </c>
+      <c r="C20" s="4">
+        <v>132</v>
+      </c>
+      <c r="D20" s="3">
+        <v>21.83</v>
+      </c>
+      <c r="E20" s="3">
+        <v>20.56</v>
+      </c>
+      <c r="F20" s="2">
+        <v>117.3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B21" s="6">
-        <v>45969</v>
-      </c>
-      <c r="C21" s="5">
-        <v>132</v>
-      </c>
-      <c r="D21" s="4">
-        <v>21.83</v>
-      </c>
-      <c r="E21" s="4">
-        <v>20.56</v>
-      </c>
-      <c r="F21" s="3">
-        <v>117.3</v>
+      <c r="A21" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="5">
+        <v>45984</v>
+      </c>
+      <c r="C21" s="4">
+        <v>147</v>
+      </c>
+      <c r="D21" s="3">
+        <v>21.42</v>
+      </c>
+      <c r="E21" s="3">
+        <v>20.13</v>
+      </c>
+      <c r="F21" s="2">
+        <v>115.5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B22" s="6">
-        <v>45984</v>
-      </c>
-      <c r="C22" s="5">
-        <v>147</v>
-      </c>
-      <c r="D22" s="4">
-        <v>21.42</v>
-      </c>
-      <c r="E22" s="4">
-        <v>20.13</v>
-      </c>
-      <c r="F22" s="3">
-        <v>115.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" s="6">
+      <c r="A22" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="5">
         <v>45982</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C22" s="4">
         <v>145</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D22" s="3">
         <v>29.24</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E22" s="3">
         <v>28.08</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F22" s="2">
         <v>2.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleaning up tagging animations for distribution
</commit_message>
<xml_diff>
--- a/tagging/data_raw/Argos_compiled.xlsx
+++ b/tagging/data_raw/Argos_compiled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretwilson/Github/emc/tagging/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDA7492-CCD4-0440-8AE6-2A0D3E5D5C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9AE40A-7127-5D49-8259-9F0D115DADCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="283833PAT" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="26354MINIPAT" sheetId="4" r:id="rId3"/>
     <sheet name="36353MINIPAT" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="181">
   <si>
     <t>PTTID</t>
   </si>
@@ -526,12 +539,6 @@
     <t>Day Since Dep</t>
   </si>
   <si>
-    <t>Surface Temp</t>
-  </si>
-  <si>
-    <t>Depth Temp</t>
-  </si>
-  <si>
     <t>2025-10-20</t>
   </si>
   <si>
@@ -570,16 +577,19 @@
   <si>
     <t>36353MINIPAT</t>
   </si>
+  <si>
+    <t>2025-11-01</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="0.0000000"/>
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="0.0000000"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -606,7 +616,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -629,41 +639,24 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,12 +964,13 @@
   <dimension ref="A1:G256"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1015,7 +1009,7 @@
       <c r="D3">
         <v>-61.879240000000003</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>45832</v>
       </c>
     </row>
@@ -1032,7 +1026,7 @@
       <c r="D4">
         <v>-61.87941</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>45838</v>
       </c>
     </row>
@@ -1049,7 +1043,7 @@
       <c r="D5">
         <v>-61.901040000000002</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>45868</v>
       </c>
     </row>
@@ -1066,7 +1060,7 @@
       <c r="D6">
         <v>-61.921990000000001</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>45873</v>
       </c>
     </row>
@@ -1083,7 +1077,7 @@
       <c r="D7">
         <v>-61.952629999999999</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>45875</v>
       </c>
     </row>
@@ -1100,7 +1094,7 @@
       <c r="D8">
         <v>-61.997</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>45894</v>
       </c>
     </row>
@@ -1117,7 +1111,7 @@
       <c r="D9">
         <v>-62.011270000000003</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>45897</v>
       </c>
     </row>
@@ -1134,7 +1128,7 @@
       <c r="D10">
         <v>-61.99633</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>45898</v>
       </c>
     </row>
@@ -1151,7 +1145,7 @@
       <c r="D11">
         <v>-61.956139999999998</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>45909</v>
       </c>
     </row>
@@ -1168,7 +1162,7 @@
       <c r="D12">
         <v>-61.918379999999999</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>45943</v>
       </c>
     </row>
@@ -6395,7 +6389,7 @@
   <dimension ref="A1:G271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6439,7 +6433,7 @@
       <c r="D3">
         <v>-61.951830000000001</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>45840</v>
       </c>
     </row>
@@ -6456,7 +6450,7 @@
       <c r="D4">
         <v>-61.981389999999998</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>45843</v>
       </c>
     </row>
@@ -6473,7 +6467,7 @@
       <c r="D5">
         <v>-61.936140000000002</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>45849</v>
       </c>
     </row>
@@ -6490,7 +6484,7 @@
       <c r="D6">
         <v>-61.934190000000001</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>45852</v>
       </c>
     </row>
@@ -6507,7 +6501,7 @@
       <c r="D7">
         <v>-61.950060000000001</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>45857</v>
       </c>
     </row>
@@ -6524,7 +6518,7 @@
       <c r="D8">
         <v>-61.993160000000003</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>45860</v>
       </c>
     </row>
@@ -6541,7 +6535,7 @@
       <c r="D9">
         <v>-62.02008</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>45865</v>
       </c>
     </row>
@@ -6558,7 +6552,7 @@
       <c r="D10">
         <v>-62.025320000000001</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>45870</v>
       </c>
     </row>
@@ -6575,7 +6569,7 @@
       <c r="D11">
         <v>-61.99371</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>45873</v>
       </c>
     </row>
@@ -6592,7 +6586,7 @@
       <c r="D12">
         <v>-61.963799999999999</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>45876</v>
       </c>
     </row>
@@ -6609,7 +6603,7 @@
       <c r="D13">
         <v>-61.983080000000001</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>45883</v>
       </c>
     </row>
@@ -6626,7 +6620,7 @@
       <c r="D14">
         <v>-61.994579999999999</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <v>45887</v>
       </c>
     </row>
@@ -6643,7 +6637,7 @@
       <c r="D15">
         <v>-61.947969999999998</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>45890</v>
       </c>
     </row>
@@ -6660,7 +6654,7 @@
       <c r="D16">
         <v>-61.90954</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>45894</v>
       </c>
     </row>
@@ -6677,7 +6671,7 @@
       <c r="D17">
         <v>-61.86092</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="8">
         <v>45897</v>
       </c>
     </row>
@@ -6694,7 +6688,7 @@
       <c r="D18">
         <v>-61.816589999999998</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <v>45900</v>
       </c>
     </row>
@@ -6711,7 +6705,7 @@
       <c r="D19">
         <v>-61.779800000000002</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>45909</v>
       </c>
     </row>
@@ -6728,7 +6722,7 @@
       <c r="D20">
         <v>-61.783790000000003</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>45912</v>
       </c>
     </row>
@@ -6745,7 +6739,7 @@
       <c r="D21">
         <v>-61.789929999999998</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <v>45915</v>
       </c>
     </row>
@@ -6762,7 +6756,7 @@
       <c r="D22">
         <v>-61.749960000000002</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <v>45918</v>
       </c>
     </row>
@@ -6779,7 +6773,7 @@
       <c r="D23">
         <v>-61.779870000000003</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <v>45921</v>
       </c>
     </row>
@@ -6796,7 +6790,7 @@
       <c r="D24">
         <v>-61.828029999999998</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>45928</v>
       </c>
     </row>
@@ -6813,7 +6807,7 @@
       <c r="D25">
         <v>-61.809019999999997</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>45931</v>
       </c>
     </row>
@@ -6830,7 +6824,7 @@
       <c r="D26">
         <v>-61.762390000000003</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>45935</v>
       </c>
     </row>
@@ -6847,7 +6841,7 @@
       <c r="D27">
         <v>-61.758629999999997</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>45940</v>
       </c>
     </row>
@@ -12071,19 +12065,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FEF50CA-A599-B44F-8ED0-C8714E499ECA}">
-  <dimension ref="A1:F137"/>
+  <dimension ref="A1:G263"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12102,7 +12096,7 @@
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -12122,8 +12116,8 @@
       <c r="D3">
         <v>-62.017498199999999</v>
       </c>
-      <c r="E3" s="11">
-        <v>45838</v>
+      <c r="E3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -12139,8 +12133,8 @@
       <c r="D4">
         <v>-62.683610399999999</v>
       </c>
-      <c r="E4" s="11">
-        <v>45848</v>
+      <c r="E4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -12156,8 +12150,8 @@
       <c r="D5">
         <v>-63.516307300000001</v>
       </c>
-      <c r="E5" s="11">
-        <v>45863</v>
+      <c r="E5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -12173,8 +12167,8 @@
       <c r="D6">
         <v>-63.269756999999998</v>
       </c>
-      <c r="E6" s="11">
-        <v>45881</v>
+      <c r="E6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -12190,8 +12184,8 @@
       <c r="D7">
         <v>-64.013177799999994</v>
       </c>
-      <c r="E7" s="11">
-        <v>45897</v>
+      <c r="E7" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -12207,8 +12201,8 @@
       <c r="D8">
         <v>-63.350789300000002</v>
       </c>
-      <c r="E8" s="11">
-        <v>45915</v>
+      <c r="E8" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -12224,8 +12218,8 @@
       <c r="D9">
         <v>-61.813349799999997</v>
       </c>
-      <c r="E9" s="11">
-        <v>45933</v>
+      <c r="E9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -12241,8 +12235,8 @@
       <c r="D10">
         <v>-62.619306600000002</v>
       </c>
-      <c r="E10" s="11">
-        <v>45962</v>
+      <c r="E10" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -12258,8 +12252,8 @@
       <c r="D11">
         <v>-63.427345099999997</v>
       </c>
-      <c r="E11" s="11">
-        <v>45982</v>
+      <c r="E11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -12278,10 +12272,10 @@
         <v>166</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>60</v>
@@ -12311,8 +12305,8 @@
       <c r="A15" t="s">
         <v>164</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
+      <c r="B15" s="10">
+        <v>45838</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -14272,7 +14266,7 @@
         <v>164</v>
       </c>
       <c r="B113" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C113">
         <v>113</v>
@@ -14292,7 +14286,7 @@
         <v>164</v>
       </c>
       <c r="B114" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C114">
         <v>115</v>
@@ -14312,7 +14306,7 @@
         <v>164</v>
       </c>
       <c r="B115" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C115">
         <v>118</v>
@@ -14332,7 +14326,7 @@
         <v>164</v>
       </c>
       <c r="B116" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C116">
         <v>121</v>
@@ -14352,7 +14346,7 @@
         <v>164</v>
       </c>
       <c r="B117" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C117">
         <v>124</v>
@@ -14372,7 +14366,7 @@
         <v>164</v>
       </c>
       <c r="B118" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C118">
         <v>127</v>
@@ -14392,7 +14386,7 @@
         <v>164</v>
       </c>
       <c r="B119" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C119">
         <v>130</v>
@@ -14412,7 +14406,7 @@
         <v>164</v>
       </c>
       <c r="B120" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C120">
         <v>134</v>
@@ -14432,7 +14426,7 @@
         <v>164</v>
       </c>
       <c r="B121" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C121">
         <v>138</v>
@@ -14452,7 +14446,7 @@
         <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C122">
         <v>142</v>
@@ -14472,7 +14466,7 @@
         <v>164</v>
       </c>
       <c r="B123" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C123">
         <v>143</v>
@@ -14492,7 +14486,7 @@
         <v>164</v>
       </c>
       <c r="B124" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C124">
         <v>143</v>
@@ -14512,7 +14506,7 @@
         <v>164</v>
       </c>
       <c r="B125" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C125">
         <v>143</v>
@@ -14532,7 +14526,7 @@
         <v>164</v>
       </c>
       <c r="B126" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C126">
         <v>144</v>
@@ -14552,7 +14546,7 @@
         <v>164</v>
       </c>
       <c r="B127" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C127">
         <v>144</v>
@@ -14572,7 +14566,7 @@
         <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C128">
         <v>144</v>
@@ -14587,12 +14581,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>164</v>
       </c>
       <c r="B129" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C129">
         <v>144</v>
@@ -14607,12 +14601,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>164</v>
       </c>
       <c r="B130" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C130">
         <v>144</v>
@@ -14627,7 +14621,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>164</v>
       </c>
@@ -14647,7 +14641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>164</v>
       </c>
@@ -14667,7 +14661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>164</v>
       </c>
@@ -14687,7 +14681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>164</v>
       </c>
@@ -14707,7 +14701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>164</v>
       </c>
@@ -14727,7 +14721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>164</v>
       </c>
@@ -14747,7 +14741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>164</v>
       </c>
@@ -14765,6 +14759,3010 @@
       </c>
       <c r="F137">
         <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G139" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>164</v>
+      </c>
+      <c r="B140" t="s">
+        <v>26</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>0.8</v>
+      </c>
+      <c r="F140">
+        <v>1.2</v>
+      </c>
+      <c r="G140">
+        <f>F140-E140</f>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>164</v>
+      </c>
+      <c r="B141" t="s">
+        <v>26</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
+      <c r="E141">
+        <v>1.6</v>
+      </c>
+      <c r="F141">
+        <v>2.4</v>
+      </c>
+      <c r="G141">
+        <f t="shared" ref="G141:G204" si="0">F141-E141</f>
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>164</v>
+      </c>
+      <c r="B142" t="s">
+        <v>26</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>4</v>
+      </c>
+      <c r="E142">
+        <v>3.2</v>
+      </c>
+      <c r="F142">
+        <v>4.8</v>
+      </c>
+      <c r="G142">
+        <f t="shared" si="0"/>
+        <v>1.5999999999999996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>164</v>
+      </c>
+      <c r="B143" t="s">
+        <v>26</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>9</v>
+      </c>
+      <c r="E143">
+        <v>7.2</v>
+      </c>
+      <c r="F143">
+        <v>10.8</v>
+      </c>
+      <c r="G143">
+        <f t="shared" si="0"/>
+        <v>3.6000000000000005</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>164</v>
+      </c>
+      <c r="B144" t="s">
+        <v>42</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144">
+        <v>12</v>
+      </c>
+      <c r="E144">
+        <v>9.6</v>
+      </c>
+      <c r="F144">
+        <v>14.4</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>164</v>
+      </c>
+      <c r="B145" t="s">
+        <v>42</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>48</v>
+      </c>
+      <c r="E145">
+        <v>38.4</v>
+      </c>
+      <c r="F145">
+        <v>57.6</v>
+      </c>
+      <c r="G145">
+        <f t="shared" si="0"/>
+        <v>19.200000000000003</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>164</v>
+      </c>
+      <c r="B146" t="s">
+        <v>43</v>
+      </c>
+      <c r="C146">
+        <v>3</v>
+      </c>
+      <c r="D146">
+        <v>66</v>
+      </c>
+      <c r="E146">
+        <v>52.8</v>
+      </c>
+      <c r="F146">
+        <v>79.2</v>
+      </c>
+      <c r="G146">
+        <f t="shared" si="0"/>
+        <v>26.400000000000006</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>164</v>
+      </c>
+      <c r="B147" t="s">
+        <v>43</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+      <c r="D147">
+        <v>101</v>
+      </c>
+      <c r="E147">
+        <v>80.8</v>
+      </c>
+      <c r="F147">
+        <v>121.2</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="0"/>
+        <v>40.400000000000006</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>164</v>
+      </c>
+      <c r="B148" t="s">
+        <v>44</v>
+      </c>
+      <c r="C148">
+        <v>4</v>
+      </c>
+      <c r="D148">
+        <v>7</v>
+      </c>
+      <c r="E148">
+        <v>5.6</v>
+      </c>
+      <c r="F148">
+        <v>8.4</v>
+      </c>
+      <c r="G148">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000007</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>164</v>
+      </c>
+      <c r="B149" t="s">
+        <v>44</v>
+      </c>
+      <c r="C149">
+        <v>4</v>
+      </c>
+      <c r="D149">
+        <v>27</v>
+      </c>
+      <c r="E149">
+        <v>21.6</v>
+      </c>
+      <c r="F149">
+        <v>32.4</v>
+      </c>
+      <c r="G149">
+        <f t="shared" si="0"/>
+        <v>10.799999999999997</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>164</v>
+      </c>
+      <c r="B150" t="s">
+        <v>45</v>
+      </c>
+      <c r="C150">
+        <v>5</v>
+      </c>
+      <c r="D150">
+        <v>52</v>
+      </c>
+      <c r="E150">
+        <v>41.6</v>
+      </c>
+      <c r="F150">
+        <v>62.4</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="0"/>
+        <v>20.799999999999997</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>164</v>
+      </c>
+      <c r="B151" t="s">
+        <v>45</v>
+      </c>
+      <c r="C151">
+        <v>5</v>
+      </c>
+      <c r="D151">
+        <v>89</v>
+      </c>
+      <c r="E151">
+        <v>71.2</v>
+      </c>
+      <c r="F151">
+        <v>106.8</v>
+      </c>
+      <c r="G151">
+        <f t="shared" si="0"/>
+        <v>35.599999999999994</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>164</v>
+      </c>
+      <c r="B152" t="s">
+        <v>45</v>
+      </c>
+      <c r="C152">
+        <v>5</v>
+      </c>
+      <c r="D152">
+        <v>115</v>
+      </c>
+      <c r="E152">
+        <v>92</v>
+      </c>
+      <c r="F152">
+        <v>138</v>
+      </c>
+      <c r="G152">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>164</v>
+      </c>
+      <c r="B153" t="s">
+        <v>46</v>
+      </c>
+      <c r="C153">
+        <v>6</v>
+      </c>
+      <c r="D153">
+        <v>31</v>
+      </c>
+      <c r="E153">
+        <v>24.8</v>
+      </c>
+      <c r="F153">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="0"/>
+        <v>12.400000000000002</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>164</v>
+      </c>
+      <c r="B154" t="s">
+        <v>47</v>
+      </c>
+      <c r="C154">
+        <v>7</v>
+      </c>
+      <c r="D154">
+        <v>18</v>
+      </c>
+      <c r="E154">
+        <v>14.4</v>
+      </c>
+      <c r="F154">
+        <v>21.6</v>
+      </c>
+      <c r="G154">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000011</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>164</v>
+      </c>
+      <c r="B155" t="s">
+        <v>48</v>
+      </c>
+      <c r="C155">
+        <v>8</v>
+      </c>
+      <c r="D155">
+        <v>74</v>
+      </c>
+      <c r="E155">
+        <v>59.2</v>
+      </c>
+      <c r="F155">
+        <v>88.8</v>
+      </c>
+      <c r="G155">
+        <f t="shared" si="0"/>
+        <v>29.599999999999994</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>164</v>
+      </c>
+      <c r="B156" t="s">
+        <v>49</v>
+      </c>
+      <c r="C156">
+        <v>9</v>
+      </c>
+      <c r="D156">
+        <v>142</v>
+      </c>
+      <c r="E156">
+        <v>113.6</v>
+      </c>
+      <c r="F156">
+        <v>170.4</v>
+      </c>
+      <c r="G156">
+        <f t="shared" si="0"/>
+        <v>56.800000000000011</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>164</v>
+      </c>
+      <c r="B157" t="s">
+        <v>50</v>
+      </c>
+      <c r="C157">
+        <v>10</v>
+      </c>
+      <c r="D157">
+        <v>11</v>
+      </c>
+      <c r="E157">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F157">
+        <v>13.2</v>
+      </c>
+      <c r="G157">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>164</v>
+      </c>
+      <c r="B158" t="s">
+        <v>51</v>
+      </c>
+      <c r="C158">
+        <v>11</v>
+      </c>
+      <c r="D158">
+        <v>63</v>
+      </c>
+      <c r="E158">
+        <v>50.4</v>
+      </c>
+      <c r="F158">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="G158">
+        <f t="shared" si="0"/>
+        <v>25.199999999999996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>164</v>
+      </c>
+      <c r="B159" t="s">
+        <v>52</v>
+      </c>
+      <c r="C159">
+        <v>12</v>
+      </c>
+      <c r="D159">
+        <v>17</v>
+      </c>
+      <c r="E159">
+        <v>13.6</v>
+      </c>
+      <c r="F159">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G159">
+        <f t="shared" si="0"/>
+        <v>6.7999999999999989</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>164</v>
+      </c>
+      <c r="B160" t="s">
+        <v>53</v>
+      </c>
+      <c r="C160">
+        <v>13</v>
+      </c>
+      <c r="D160">
+        <v>34</v>
+      </c>
+      <c r="E160">
+        <v>27.2</v>
+      </c>
+      <c r="F160">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="G160">
+        <f t="shared" si="0"/>
+        <v>13.599999999999998</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>164</v>
+      </c>
+      <c r="B161" t="s">
+        <v>53</v>
+      </c>
+      <c r="C161">
+        <v>13</v>
+      </c>
+      <c r="D161">
+        <v>52</v>
+      </c>
+      <c r="E161">
+        <v>41.6</v>
+      </c>
+      <c r="F161">
+        <v>62.4</v>
+      </c>
+      <c r="G161">
+        <f t="shared" si="0"/>
+        <v>20.799999999999997</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" t="s">
+        <v>54</v>
+      </c>
+      <c r="C162">
+        <v>14</v>
+      </c>
+      <c r="D162">
+        <v>78</v>
+      </c>
+      <c r="E162">
+        <v>62.4</v>
+      </c>
+      <c r="F162">
+        <v>93.6</v>
+      </c>
+      <c r="G162">
+        <f t="shared" si="0"/>
+        <v>31.199999999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>164</v>
+      </c>
+      <c r="B163" t="s">
+        <v>54</v>
+      </c>
+      <c r="C163">
+        <v>14</v>
+      </c>
+      <c r="D163">
+        <v>104</v>
+      </c>
+      <c r="E163">
+        <v>83.2</v>
+      </c>
+      <c r="F163">
+        <v>124.8</v>
+      </c>
+      <c r="G163">
+        <f t="shared" si="0"/>
+        <v>41.599999999999994</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" t="s">
+        <v>55</v>
+      </c>
+      <c r="C164">
+        <v>15</v>
+      </c>
+      <c r="D164">
+        <v>141</v>
+      </c>
+      <c r="E164">
+        <v>112.8</v>
+      </c>
+      <c r="F164">
+        <v>169.2</v>
+      </c>
+      <c r="G164">
+        <f t="shared" si="0"/>
+        <v>56.399999999999991</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>164</v>
+      </c>
+      <c r="B165" t="s">
+        <v>56</v>
+      </c>
+      <c r="C165">
+        <v>16</v>
+      </c>
+      <c r="D165">
+        <v>18</v>
+      </c>
+      <c r="E165">
+        <v>14.4</v>
+      </c>
+      <c r="F165">
+        <v>21.6</v>
+      </c>
+      <c r="G165">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000011</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>164</v>
+      </c>
+      <c r="B166" t="s">
+        <v>57</v>
+      </c>
+      <c r="C166">
+        <v>17</v>
+      </c>
+      <c r="D166">
+        <v>6</v>
+      </c>
+      <c r="E166">
+        <v>4.8</v>
+      </c>
+      <c r="F166">
+        <v>7.2</v>
+      </c>
+      <c r="G166">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>164</v>
+      </c>
+      <c r="B167" t="s">
+        <v>64</v>
+      </c>
+      <c r="C167">
+        <v>18</v>
+      </c>
+      <c r="D167">
+        <v>111</v>
+      </c>
+      <c r="E167">
+        <v>88.8</v>
+      </c>
+      <c r="F167">
+        <v>133.19999999999999</v>
+      </c>
+      <c r="G167">
+        <f t="shared" si="0"/>
+        <v>44.399999999999991</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>164</v>
+      </c>
+      <c r="B168" t="s">
+        <v>65</v>
+      </c>
+      <c r="C168">
+        <v>19</v>
+      </c>
+      <c r="D168">
+        <v>45</v>
+      </c>
+      <c r="E168">
+        <v>36</v>
+      </c>
+      <c r="F168">
+        <v>54</v>
+      </c>
+      <c r="G168">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>164</v>
+      </c>
+      <c r="B169" t="s">
+        <v>66</v>
+      </c>
+      <c r="C169">
+        <v>20</v>
+      </c>
+      <c r="D169">
+        <v>134</v>
+      </c>
+      <c r="E169">
+        <v>107.2</v>
+      </c>
+      <c r="F169">
+        <v>160.80000000000001</v>
+      </c>
+      <c r="G169">
+        <f t="shared" si="0"/>
+        <v>53.600000000000009</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>164</v>
+      </c>
+      <c r="B170" t="s">
+        <v>69</v>
+      </c>
+      <c r="C170">
+        <v>23</v>
+      </c>
+      <c r="D170">
+        <v>59</v>
+      </c>
+      <c r="E170">
+        <v>47.2</v>
+      </c>
+      <c r="F170">
+        <v>70.8</v>
+      </c>
+      <c r="G170">
+        <f t="shared" si="0"/>
+        <v>23.599999999999994</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>164</v>
+      </c>
+      <c r="B171" t="s">
+        <v>70</v>
+      </c>
+      <c r="C171">
+        <v>24</v>
+      </c>
+      <c r="D171">
+        <v>92</v>
+      </c>
+      <c r="E171">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="F171">
+        <v>110.4</v>
+      </c>
+      <c r="G171">
+        <f t="shared" si="0"/>
+        <v>36.800000000000011</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>164</v>
+      </c>
+      <c r="B172" t="s">
+        <v>71</v>
+      </c>
+      <c r="C172">
+        <v>25</v>
+      </c>
+      <c r="D172">
+        <v>11</v>
+      </c>
+      <c r="E172">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F172">
+        <v>13.2</v>
+      </c>
+      <c r="G172">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>164</v>
+      </c>
+      <c r="B173" t="s">
+        <v>72</v>
+      </c>
+      <c r="C173">
+        <v>26</v>
+      </c>
+      <c r="D173">
+        <v>67</v>
+      </c>
+      <c r="E173">
+        <v>53.6</v>
+      </c>
+      <c r="F173">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="G173">
+        <f t="shared" si="0"/>
+        <v>26.800000000000004</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>164</v>
+      </c>
+      <c r="B174" t="s">
+        <v>73</v>
+      </c>
+      <c r="C174">
+        <v>27</v>
+      </c>
+      <c r="D174">
+        <v>14</v>
+      </c>
+      <c r="E174">
+        <v>11.2</v>
+      </c>
+      <c r="F174">
+        <v>16.8</v>
+      </c>
+      <c r="G174">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000014</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>164</v>
+      </c>
+      <c r="B175" t="s">
+        <v>74</v>
+      </c>
+      <c r="C175">
+        <v>28</v>
+      </c>
+      <c r="D175">
+        <v>36</v>
+      </c>
+      <c r="E175">
+        <v>28.8</v>
+      </c>
+      <c r="F175">
+        <v>43.2</v>
+      </c>
+      <c r="G175">
+        <f t="shared" si="0"/>
+        <v>14.400000000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>164</v>
+      </c>
+      <c r="B176" t="s">
+        <v>75</v>
+      </c>
+      <c r="C176">
+        <v>29</v>
+      </c>
+      <c r="D176">
+        <v>62</v>
+      </c>
+      <c r="E176">
+        <v>49.6</v>
+      </c>
+      <c r="F176">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="G176">
+        <f t="shared" si="0"/>
+        <v>24.800000000000004</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>164</v>
+      </c>
+      <c r="B177" t="s">
+        <v>75</v>
+      </c>
+      <c r="C177">
+        <v>29</v>
+      </c>
+      <c r="D177">
+        <v>103</v>
+      </c>
+      <c r="E177">
+        <v>82.4</v>
+      </c>
+      <c r="F177">
+        <v>123.6</v>
+      </c>
+      <c r="G177">
+        <f t="shared" si="0"/>
+        <v>41.199999999999989</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>164</v>
+      </c>
+      <c r="B178" t="s">
+        <v>76</v>
+      </c>
+      <c r="C178">
+        <v>30</v>
+      </c>
+      <c r="D178">
+        <v>143</v>
+      </c>
+      <c r="E178">
+        <v>114.4</v>
+      </c>
+      <c r="F178">
+        <v>171.6</v>
+      </c>
+      <c r="G178">
+        <f t="shared" si="0"/>
+        <v>57.199999999999989</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>164</v>
+      </c>
+      <c r="B179" t="s">
+        <v>77</v>
+      </c>
+      <c r="C179">
+        <v>31</v>
+      </c>
+      <c r="D179">
+        <v>11</v>
+      </c>
+      <c r="E179">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F179">
+        <v>13.2</v>
+      </c>
+      <c r="G179">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>164</v>
+      </c>
+      <c r="B180" t="s">
+        <v>78</v>
+      </c>
+      <c r="C180">
+        <v>32</v>
+      </c>
+      <c r="D180">
+        <v>77</v>
+      </c>
+      <c r="E180">
+        <v>61.6</v>
+      </c>
+      <c r="F180">
+        <v>92.4</v>
+      </c>
+      <c r="G180">
+        <f t="shared" si="0"/>
+        <v>30.800000000000004</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>164</v>
+      </c>
+      <c r="B181" t="s">
+        <v>79</v>
+      </c>
+      <c r="C181">
+        <v>33</v>
+      </c>
+      <c r="D181">
+        <v>54</v>
+      </c>
+      <c r="E181">
+        <v>43.2</v>
+      </c>
+      <c r="F181">
+        <v>64.8</v>
+      </c>
+      <c r="G181">
+        <f t="shared" si="0"/>
+        <v>21.599999999999994</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>164</v>
+      </c>
+      <c r="B182" t="s">
+        <v>80</v>
+      </c>
+      <c r="C182">
+        <v>34</v>
+      </c>
+      <c r="D182">
+        <v>91</v>
+      </c>
+      <c r="E182">
+        <v>72.8</v>
+      </c>
+      <c r="F182">
+        <v>109.2</v>
+      </c>
+      <c r="G182">
+        <f t="shared" si="0"/>
+        <v>36.400000000000006</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>164</v>
+      </c>
+      <c r="B183" t="s">
+        <v>82</v>
+      </c>
+      <c r="C183">
+        <v>36</v>
+      </c>
+      <c r="D183">
+        <v>122</v>
+      </c>
+      <c r="E183">
+        <v>97.6</v>
+      </c>
+      <c r="F183">
+        <v>146.4</v>
+      </c>
+      <c r="G183">
+        <f t="shared" si="0"/>
+        <v>48.800000000000011</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>164</v>
+      </c>
+      <c r="B184" t="s">
+        <v>85</v>
+      </c>
+      <c r="C184">
+        <v>39</v>
+      </c>
+      <c r="D184">
+        <v>18</v>
+      </c>
+      <c r="E184">
+        <v>14.4</v>
+      </c>
+      <c r="F184">
+        <v>21.6</v>
+      </c>
+      <c r="G184">
+        <f t="shared" si="0"/>
+        <v>7.2000000000000011</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>164</v>
+      </c>
+      <c r="B185" t="s">
+        <v>86</v>
+      </c>
+      <c r="C185">
+        <v>40</v>
+      </c>
+      <c r="D185">
+        <v>7</v>
+      </c>
+      <c r="E185">
+        <v>5.6</v>
+      </c>
+      <c r="F185">
+        <v>8.4</v>
+      </c>
+      <c r="G185">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000007</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>164</v>
+      </c>
+      <c r="B186" t="s">
+        <v>87</v>
+      </c>
+      <c r="C186">
+        <v>41</v>
+      </c>
+      <c r="D186">
+        <v>134</v>
+      </c>
+      <c r="E186">
+        <v>107.2</v>
+      </c>
+      <c r="F186">
+        <v>160.80000000000001</v>
+      </c>
+      <c r="G186">
+        <f t="shared" si="0"/>
+        <v>53.600000000000009</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>164</v>
+      </c>
+      <c r="B187" t="s">
+        <v>89</v>
+      </c>
+      <c r="C187">
+        <v>43</v>
+      </c>
+      <c r="D187">
+        <v>43</v>
+      </c>
+      <c r="E187">
+        <v>34.4</v>
+      </c>
+      <c r="F187">
+        <v>51.6</v>
+      </c>
+      <c r="G187">
+        <f t="shared" si="0"/>
+        <v>17.200000000000003</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>164</v>
+      </c>
+      <c r="B188" t="s">
+        <v>90</v>
+      </c>
+      <c r="C188">
+        <v>44</v>
+      </c>
+      <c r="D188">
+        <v>63</v>
+      </c>
+      <c r="E188">
+        <v>50.4</v>
+      </c>
+      <c r="F188">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="G188">
+        <f t="shared" si="0"/>
+        <v>25.199999999999996</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>164</v>
+      </c>
+      <c r="B189" t="s">
+        <v>91</v>
+      </c>
+      <c r="C189">
+        <v>45</v>
+      </c>
+      <c r="D189">
+        <v>19</v>
+      </c>
+      <c r="E189">
+        <v>15.2</v>
+      </c>
+      <c r="F189">
+        <v>22.8</v>
+      </c>
+      <c r="G189">
+        <f t="shared" si="0"/>
+        <v>7.6000000000000014</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>164</v>
+      </c>
+      <c r="B190" t="s">
+        <v>92</v>
+      </c>
+      <c r="C190">
+        <v>46</v>
+      </c>
+      <c r="D190">
+        <v>44</v>
+      </c>
+      <c r="E190">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="F190">
+        <v>52.8</v>
+      </c>
+      <c r="G190">
+        <f t="shared" si="0"/>
+        <v>17.599999999999994</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>164</v>
+      </c>
+      <c r="B191" t="s">
+        <v>93</v>
+      </c>
+      <c r="C191">
+        <v>47</v>
+      </c>
+      <c r="D191">
+        <v>72</v>
+      </c>
+      <c r="E191">
+        <v>57.6</v>
+      </c>
+      <c r="F191">
+        <v>86.4</v>
+      </c>
+      <c r="G191">
+        <f t="shared" si="0"/>
+        <v>28.800000000000004</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>164</v>
+      </c>
+      <c r="B192" t="s">
+        <v>93</v>
+      </c>
+      <c r="C192">
+        <v>47</v>
+      </c>
+      <c r="D192">
+        <v>101</v>
+      </c>
+      <c r="E192">
+        <v>80.8</v>
+      </c>
+      <c r="F192">
+        <v>121.2</v>
+      </c>
+      <c r="G192">
+        <f t="shared" si="0"/>
+        <v>40.400000000000006</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>164</v>
+      </c>
+      <c r="B193" t="s">
+        <v>94</v>
+      </c>
+      <c r="C193">
+        <v>48</v>
+      </c>
+      <c r="D193">
+        <v>144</v>
+      </c>
+      <c r="E193">
+        <v>115.2</v>
+      </c>
+      <c r="F193">
+        <v>172.8</v>
+      </c>
+      <c r="G193">
+        <f t="shared" si="0"/>
+        <v>57.600000000000009</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>164</v>
+      </c>
+      <c r="B194" t="s">
+        <v>95</v>
+      </c>
+      <c r="C194">
+        <v>49</v>
+      </c>
+      <c r="D194">
+        <v>8</v>
+      </c>
+      <c r="E194">
+        <v>6.4</v>
+      </c>
+      <c r="F194">
+        <v>9.6</v>
+      </c>
+      <c r="G194">
+        <f t="shared" si="0"/>
+        <v>3.1999999999999993</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>164</v>
+      </c>
+      <c r="B195" t="s">
+        <v>96</v>
+      </c>
+      <c r="C195">
+        <v>50</v>
+      </c>
+      <c r="D195">
+        <v>58</v>
+      </c>
+      <c r="E195">
+        <v>46.4</v>
+      </c>
+      <c r="F195">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="G195">
+        <f t="shared" si="0"/>
+        <v>23.199999999999996</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>164</v>
+      </c>
+      <c r="B196" t="s">
+        <v>99</v>
+      </c>
+      <c r="C196">
+        <v>53</v>
+      </c>
+      <c r="D196">
+        <v>132</v>
+      </c>
+      <c r="E196">
+        <v>105.6</v>
+      </c>
+      <c r="F196">
+        <v>158.4</v>
+      </c>
+      <c r="G196">
+        <f t="shared" si="0"/>
+        <v>52.800000000000011</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>164</v>
+      </c>
+      <c r="B197" t="s">
+        <v>100</v>
+      </c>
+      <c r="C197">
+        <v>54</v>
+      </c>
+      <c r="D197">
+        <v>97</v>
+      </c>
+      <c r="E197">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="F197">
+        <v>116.4</v>
+      </c>
+      <c r="G197">
+        <f t="shared" si="0"/>
+        <v>38.800000000000011</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>164</v>
+      </c>
+      <c r="B198" t="s">
+        <v>101</v>
+      </c>
+      <c r="C198">
+        <v>55</v>
+      </c>
+      <c r="D198">
+        <v>11</v>
+      </c>
+      <c r="E198">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F198">
+        <v>13.2</v>
+      </c>
+      <c r="G198">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>164</v>
+      </c>
+      <c r="B199" t="s">
+        <v>102</v>
+      </c>
+      <c r="C199">
+        <v>56</v>
+      </c>
+      <c r="D199">
+        <v>43</v>
+      </c>
+      <c r="E199">
+        <v>34.4</v>
+      </c>
+      <c r="F199">
+        <v>51.6</v>
+      </c>
+      <c r="G199">
+        <f t="shared" si="0"/>
+        <v>17.200000000000003</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>164</v>
+      </c>
+      <c r="B200" t="s">
+        <v>103</v>
+      </c>
+      <c r="C200">
+        <v>57</v>
+      </c>
+      <c r="D200">
+        <v>68</v>
+      </c>
+      <c r="E200">
+        <v>54.4</v>
+      </c>
+      <c r="F200">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="G200">
+        <f t="shared" si="0"/>
+        <v>27.199999999999996</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>164</v>
+      </c>
+      <c r="B201" t="s">
+        <v>104</v>
+      </c>
+      <c r="C201">
+        <v>58</v>
+      </c>
+      <c r="D201">
+        <v>112</v>
+      </c>
+      <c r="E201">
+        <v>89.6</v>
+      </c>
+      <c r="F201">
+        <v>134.4</v>
+      </c>
+      <c r="G201">
+        <f t="shared" si="0"/>
+        <v>44.800000000000011</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>164</v>
+      </c>
+      <c r="B202" t="s">
+        <v>105</v>
+      </c>
+      <c r="C202">
+        <v>59</v>
+      </c>
+      <c r="D202">
+        <v>27</v>
+      </c>
+      <c r="E202">
+        <v>21.6</v>
+      </c>
+      <c r="F202">
+        <v>32.4</v>
+      </c>
+      <c r="G202">
+        <f t="shared" si="0"/>
+        <v>10.799999999999997</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>164</v>
+      </c>
+      <c r="B203" t="s">
+        <v>106</v>
+      </c>
+      <c r="C203">
+        <v>60</v>
+      </c>
+      <c r="D203">
+        <v>6</v>
+      </c>
+      <c r="E203">
+        <v>4.8</v>
+      </c>
+      <c r="F203">
+        <v>7.2</v>
+      </c>
+      <c r="G203">
+        <f t="shared" si="0"/>
+        <v>2.4000000000000004</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>164</v>
+      </c>
+      <c r="B204" t="s">
+        <v>107</v>
+      </c>
+      <c r="C204">
+        <v>61</v>
+      </c>
+      <c r="D204">
+        <v>21</v>
+      </c>
+      <c r="E204">
+        <v>16.8</v>
+      </c>
+      <c r="F204">
+        <v>25.2</v>
+      </c>
+      <c r="G204">
+        <f t="shared" si="0"/>
+        <v>8.3999999999999986</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>164</v>
+      </c>
+      <c r="B205" t="s">
+        <v>108</v>
+      </c>
+      <c r="C205">
+        <v>62</v>
+      </c>
+      <c r="D205">
+        <v>51</v>
+      </c>
+      <c r="E205">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="F205">
+        <v>61.2</v>
+      </c>
+      <c r="G205">
+        <f t="shared" ref="G205:G263" si="1">F205-E205</f>
+        <v>20.400000000000006</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>164</v>
+      </c>
+      <c r="B206" t="s">
+        <v>109</v>
+      </c>
+      <c r="C206">
+        <v>63</v>
+      </c>
+      <c r="D206">
+        <v>74</v>
+      </c>
+      <c r="E206">
+        <v>59.2</v>
+      </c>
+      <c r="F206">
+        <v>88.8</v>
+      </c>
+      <c r="G206">
+        <f t="shared" si="1"/>
+        <v>29.599999999999994</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>164</v>
+      </c>
+      <c r="B207" t="s">
+        <v>111</v>
+      </c>
+      <c r="C207">
+        <v>65</v>
+      </c>
+      <c r="D207">
+        <v>118</v>
+      </c>
+      <c r="E207">
+        <v>94.4</v>
+      </c>
+      <c r="F207">
+        <v>141.6</v>
+      </c>
+      <c r="G207">
+        <f t="shared" si="1"/>
+        <v>47.199999999999989</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>164</v>
+      </c>
+      <c r="B208" t="s">
+        <v>113</v>
+      </c>
+      <c r="C208">
+        <v>67</v>
+      </c>
+      <c r="D208">
+        <v>132</v>
+      </c>
+      <c r="E208">
+        <v>105.6</v>
+      </c>
+      <c r="F208">
+        <v>158.4</v>
+      </c>
+      <c r="G208">
+        <f t="shared" si="1"/>
+        <v>52.800000000000011</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>164</v>
+      </c>
+      <c r="B209" t="s">
+        <v>114</v>
+      </c>
+      <c r="C209">
+        <v>68</v>
+      </c>
+      <c r="D209">
+        <v>16</v>
+      </c>
+      <c r="E209">
+        <v>12.8</v>
+      </c>
+      <c r="F209">
+        <v>19.2</v>
+      </c>
+      <c r="G209">
+        <f t="shared" si="1"/>
+        <v>6.3999999999999986</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>164</v>
+      </c>
+      <c r="B210" t="s">
+        <v>116</v>
+      </c>
+      <c r="C210">
+        <v>70</v>
+      </c>
+      <c r="D210">
+        <v>43</v>
+      </c>
+      <c r="E210">
+        <v>34.4</v>
+      </c>
+      <c r="F210">
+        <v>51.6</v>
+      </c>
+      <c r="G210">
+        <f t="shared" si="1"/>
+        <v>17.200000000000003</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>164</v>
+      </c>
+      <c r="B211" t="s">
+        <v>119</v>
+      </c>
+      <c r="C211">
+        <v>73</v>
+      </c>
+      <c r="D211">
+        <v>154</v>
+      </c>
+      <c r="E211">
+        <v>123.2</v>
+      </c>
+      <c r="F211">
+        <v>184.8</v>
+      </c>
+      <c r="G211">
+        <f t="shared" si="1"/>
+        <v>61.600000000000009</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>164</v>
+      </c>
+      <c r="B212" t="s">
+        <v>121</v>
+      </c>
+      <c r="C212">
+        <v>75</v>
+      </c>
+      <c r="D212">
+        <v>96</v>
+      </c>
+      <c r="E212">
+        <v>76.8</v>
+      </c>
+      <c r="F212">
+        <v>115.2</v>
+      </c>
+      <c r="G212">
+        <f t="shared" si="1"/>
+        <v>38.400000000000006</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>164</v>
+      </c>
+      <c r="B213" t="s">
+        <v>124</v>
+      </c>
+      <c r="C213">
+        <v>78</v>
+      </c>
+      <c r="D213">
+        <v>77</v>
+      </c>
+      <c r="E213">
+        <v>61.6</v>
+      </c>
+      <c r="F213">
+        <v>92.4</v>
+      </c>
+      <c r="G213">
+        <f t="shared" si="1"/>
+        <v>30.800000000000004</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>164</v>
+      </c>
+      <c r="B214" t="s">
+        <v>126</v>
+      </c>
+      <c r="C214">
+        <v>80</v>
+      </c>
+      <c r="D214">
+        <v>54</v>
+      </c>
+      <c r="E214">
+        <v>43.2</v>
+      </c>
+      <c r="F214">
+        <v>64.8</v>
+      </c>
+      <c r="G214">
+        <f t="shared" si="1"/>
+        <v>21.599999999999994</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>164</v>
+      </c>
+      <c r="B215" t="s">
+        <v>127</v>
+      </c>
+      <c r="C215">
+        <v>81</v>
+      </c>
+      <c r="D215">
+        <v>29</v>
+      </c>
+      <c r="E215">
+        <v>23.2</v>
+      </c>
+      <c r="F215">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="G215">
+        <f t="shared" si="1"/>
+        <v>11.599999999999998</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>164</v>
+      </c>
+      <c r="B216" t="s">
+        <v>129</v>
+      </c>
+      <c r="C216">
+        <v>83</v>
+      </c>
+      <c r="D216">
+        <v>12</v>
+      </c>
+      <c r="E216">
+        <v>9.6</v>
+      </c>
+      <c r="F216">
+        <v>14.4</v>
+      </c>
+      <c r="G216">
+        <f t="shared" si="1"/>
+        <v>4.8000000000000007</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>164</v>
+      </c>
+      <c r="B217" t="s">
+        <v>131</v>
+      </c>
+      <c r="C217">
+        <v>85</v>
+      </c>
+      <c r="D217">
+        <v>144</v>
+      </c>
+      <c r="E217">
+        <v>115.2</v>
+      </c>
+      <c r="F217">
+        <v>172.8</v>
+      </c>
+      <c r="G217">
+        <f t="shared" si="1"/>
+        <v>57.600000000000009</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>164</v>
+      </c>
+      <c r="B218" t="s">
+        <v>134</v>
+      </c>
+      <c r="C218">
+        <v>88</v>
+      </c>
+      <c r="D218">
+        <v>33</v>
+      </c>
+      <c r="E218">
+        <v>26.4</v>
+      </c>
+      <c r="F218">
+        <v>39.6</v>
+      </c>
+      <c r="G218">
+        <f t="shared" si="1"/>
+        <v>13.200000000000003</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>164</v>
+      </c>
+      <c r="B219" t="s">
+        <v>135</v>
+      </c>
+      <c r="C219">
+        <v>89</v>
+      </c>
+      <c r="D219">
+        <v>14</v>
+      </c>
+      <c r="E219">
+        <v>11.2</v>
+      </c>
+      <c r="F219">
+        <v>16.8</v>
+      </c>
+      <c r="G219">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000014</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>164</v>
+      </c>
+      <c r="B220" t="s">
+        <v>135</v>
+      </c>
+      <c r="C220">
+        <v>89</v>
+      </c>
+      <c r="D220">
+        <v>38</v>
+      </c>
+      <c r="E220">
+        <v>30.4</v>
+      </c>
+      <c r="F220">
+        <v>45.6</v>
+      </c>
+      <c r="G220">
+        <f t="shared" si="1"/>
+        <v>15.200000000000003</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>164</v>
+      </c>
+      <c r="B221" t="s">
+        <v>136</v>
+      </c>
+      <c r="C221">
+        <v>90</v>
+      </c>
+      <c r="D221">
+        <v>71</v>
+      </c>
+      <c r="E221">
+        <v>56.8</v>
+      </c>
+      <c r="F221">
+        <v>85.2</v>
+      </c>
+      <c r="G221">
+        <f t="shared" si="1"/>
+        <v>28.400000000000006</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>164</v>
+      </c>
+      <c r="B222" t="s">
+        <v>136</v>
+      </c>
+      <c r="C222">
+        <v>90</v>
+      </c>
+      <c r="D222">
+        <v>103</v>
+      </c>
+      <c r="E222">
+        <v>82.4</v>
+      </c>
+      <c r="F222">
+        <v>123.6</v>
+      </c>
+      <c r="G222">
+        <f t="shared" si="1"/>
+        <v>41.199999999999989</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>164</v>
+      </c>
+      <c r="B223" t="s">
+        <v>138</v>
+      </c>
+      <c r="C223">
+        <v>92</v>
+      </c>
+      <c r="D223">
+        <v>147</v>
+      </c>
+      <c r="E223">
+        <v>117.6</v>
+      </c>
+      <c r="F223">
+        <v>176.4</v>
+      </c>
+      <c r="G223">
+        <f t="shared" si="1"/>
+        <v>58.800000000000011</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>164</v>
+      </c>
+      <c r="B224" t="s">
+        <v>139</v>
+      </c>
+      <c r="C224">
+        <v>93</v>
+      </c>
+      <c r="D224">
+        <v>9</v>
+      </c>
+      <c r="E224">
+        <v>7.2</v>
+      </c>
+      <c r="F224">
+        <v>10.8</v>
+      </c>
+      <c r="G224">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000005</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>164</v>
+      </c>
+      <c r="B225" t="s">
+        <v>140</v>
+      </c>
+      <c r="C225">
+        <v>94</v>
+      </c>
+      <c r="D225">
+        <v>55</v>
+      </c>
+      <c r="E225">
+        <v>44</v>
+      </c>
+      <c r="F225">
+        <v>66</v>
+      </c>
+      <c r="G225">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>164</v>
+      </c>
+      <c r="B226" t="s">
+        <v>142</v>
+      </c>
+      <c r="C226">
+        <v>96</v>
+      </c>
+      <c r="D226">
+        <v>89</v>
+      </c>
+      <c r="E226">
+        <v>71.2</v>
+      </c>
+      <c r="F226">
+        <v>106.8</v>
+      </c>
+      <c r="G226">
+        <f t="shared" si="1"/>
+        <v>35.599999999999994</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>164</v>
+      </c>
+      <c r="B227" t="s">
+        <v>144</v>
+      </c>
+      <c r="C227">
+        <v>98</v>
+      </c>
+      <c r="D227">
+        <v>121</v>
+      </c>
+      <c r="E227">
+        <v>96.8</v>
+      </c>
+      <c r="F227">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="G227">
+        <f t="shared" si="1"/>
+        <v>48.399999999999991</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>164</v>
+      </c>
+      <c r="B228" t="s">
+        <v>145</v>
+      </c>
+      <c r="C228">
+        <v>99</v>
+      </c>
+      <c r="D228">
+        <v>17</v>
+      </c>
+      <c r="E228">
+        <v>13.6</v>
+      </c>
+      <c r="F228">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="G228">
+        <f t="shared" si="1"/>
+        <v>6.7999999999999989</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>164</v>
+      </c>
+      <c r="B229" t="s">
+        <v>146</v>
+      </c>
+      <c r="C229">
+        <v>100</v>
+      </c>
+      <c r="D229">
+        <v>39</v>
+      </c>
+      <c r="E229">
+        <v>31.2</v>
+      </c>
+      <c r="F229">
+        <v>46.8</v>
+      </c>
+      <c r="G229">
+        <f t="shared" si="1"/>
+        <v>15.599999999999998</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>164</v>
+      </c>
+      <c r="B230" t="s">
+        <v>147</v>
+      </c>
+      <c r="C230">
+        <v>101</v>
+      </c>
+      <c r="D230">
+        <v>72</v>
+      </c>
+      <c r="E230">
+        <v>57.6</v>
+      </c>
+      <c r="F230">
+        <v>86.4</v>
+      </c>
+      <c r="G230">
+        <f t="shared" si="1"/>
+        <v>28.800000000000004</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>164</v>
+      </c>
+      <c r="B231" t="s">
+        <v>148</v>
+      </c>
+      <c r="C231">
+        <v>102</v>
+      </c>
+      <c r="D231">
+        <v>11</v>
+      </c>
+      <c r="E231">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F231">
+        <v>13.2</v>
+      </c>
+      <c r="G231">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>164</v>
+      </c>
+      <c r="B232" t="s">
+        <v>148</v>
+      </c>
+      <c r="C232">
+        <v>102</v>
+      </c>
+      <c r="D232">
+        <v>140</v>
+      </c>
+      <c r="E232">
+        <v>112</v>
+      </c>
+      <c r="F232">
+        <v>168</v>
+      </c>
+      <c r="G232">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>164</v>
+      </c>
+      <c r="B233" t="s">
+        <v>149</v>
+      </c>
+      <c r="C233">
+        <v>103</v>
+      </c>
+      <c r="D233">
+        <v>63</v>
+      </c>
+      <c r="E233">
+        <v>50.4</v>
+      </c>
+      <c r="F233">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="G233">
+        <f t="shared" si="1"/>
+        <v>25.199999999999996</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>164</v>
+      </c>
+      <c r="B234" t="s">
+        <v>150</v>
+      </c>
+      <c r="C234">
+        <v>104</v>
+      </c>
+      <c r="D234">
+        <v>18</v>
+      </c>
+      <c r="E234">
+        <v>14.4</v>
+      </c>
+      <c r="F234">
+        <v>21.6</v>
+      </c>
+      <c r="G234">
+        <f t="shared" si="1"/>
+        <v>7.2000000000000011</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>164</v>
+      </c>
+      <c r="B235" t="s">
+        <v>152</v>
+      </c>
+      <c r="C235">
+        <v>106</v>
+      </c>
+      <c r="D235">
+        <v>48</v>
+      </c>
+      <c r="E235">
+        <v>38.4</v>
+      </c>
+      <c r="F235">
+        <v>57.6</v>
+      </c>
+      <c r="G235">
+        <f t="shared" si="1"/>
+        <v>19.200000000000003</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>164</v>
+      </c>
+      <c r="B236" t="s">
+        <v>153</v>
+      </c>
+      <c r="C236">
+        <v>107</v>
+      </c>
+      <c r="D236">
+        <v>76</v>
+      </c>
+      <c r="E236">
+        <v>60.8</v>
+      </c>
+      <c r="F236">
+        <v>91.2</v>
+      </c>
+      <c r="G236">
+        <f t="shared" si="1"/>
+        <v>30.400000000000006</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>164</v>
+      </c>
+      <c r="B237" t="s">
+        <v>155</v>
+      </c>
+      <c r="C237">
+        <v>109</v>
+      </c>
+      <c r="D237">
+        <v>113</v>
+      </c>
+      <c r="E237">
+        <v>90.4</v>
+      </c>
+      <c r="F237">
+        <v>135.6</v>
+      </c>
+      <c r="G237">
+        <f t="shared" si="1"/>
+        <v>45.199999999999989</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>164</v>
+      </c>
+      <c r="B238" t="s">
+        <v>157</v>
+      </c>
+      <c r="C238">
+        <v>111</v>
+      </c>
+      <c r="D238">
+        <v>156</v>
+      </c>
+      <c r="E238">
+        <v>124.8</v>
+      </c>
+      <c r="F238">
+        <v>187.2</v>
+      </c>
+      <c r="G238">
+        <f t="shared" si="1"/>
+        <v>62.399999999999991</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>164</v>
+      </c>
+      <c r="B239" t="s">
+        <v>167</v>
+      </c>
+      <c r="C239">
+        <v>113</v>
+      </c>
+      <c r="D239">
+        <v>9</v>
+      </c>
+      <c r="E239">
+        <v>7.2</v>
+      </c>
+      <c r="F239">
+        <v>10.8</v>
+      </c>
+      <c r="G239">
+        <f t="shared" si="1"/>
+        <v>3.6000000000000005</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>164</v>
+      </c>
+      <c r="B240" t="s">
+        <v>168</v>
+      </c>
+      <c r="C240">
+        <v>115</v>
+      </c>
+      <c r="D240">
+        <v>54</v>
+      </c>
+      <c r="E240">
+        <v>43.2</v>
+      </c>
+      <c r="F240">
+        <v>64.8</v>
+      </c>
+      <c r="G240">
+        <f t="shared" si="1"/>
+        <v>21.599999999999994</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>164</v>
+      </c>
+      <c r="B241" t="s">
+        <v>169</v>
+      </c>
+      <c r="C241">
+        <v>118</v>
+      </c>
+      <c r="D241">
+        <v>88</v>
+      </c>
+      <c r="E241">
+        <v>70.400000000000006</v>
+      </c>
+      <c r="F241">
+        <v>105.6</v>
+      </c>
+      <c r="G241">
+        <f t="shared" si="1"/>
+        <v>35.199999999999989</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>164</v>
+      </c>
+      <c r="B242" t="s">
+        <v>170</v>
+      </c>
+      <c r="C242">
+        <v>121</v>
+      </c>
+      <c r="D242">
+        <v>142</v>
+      </c>
+      <c r="E242">
+        <v>113.6</v>
+      </c>
+      <c r="F242">
+        <v>170.4</v>
+      </c>
+      <c r="G242">
+        <f t="shared" si="1"/>
+        <v>56.800000000000011</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>164</v>
+      </c>
+      <c r="B243" t="s">
+        <v>171</v>
+      </c>
+      <c r="C243">
+        <v>124</v>
+      </c>
+      <c r="D243">
+        <v>121</v>
+      </c>
+      <c r="E243">
+        <v>96.8</v>
+      </c>
+      <c r="F243">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="G243">
+        <f t="shared" si="1"/>
+        <v>48.399999999999991</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>164</v>
+      </c>
+      <c r="B244" t="s">
+        <v>172</v>
+      </c>
+      <c r="C244">
+        <v>127</v>
+      </c>
+      <c r="D244">
+        <v>67</v>
+      </c>
+      <c r="E244">
+        <v>53.6</v>
+      </c>
+      <c r="F244">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="G244">
+        <f t="shared" si="1"/>
+        <v>26.800000000000004</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>164</v>
+      </c>
+      <c r="B245" t="s">
+        <v>173</v>
+      </c>
+      <c r="C245">
+        <v>130</v>
+      </c>
+      <c r="D245">
+        <v>33</v>
+      </c>
+      <c r="E245">
+        <v>26.4</v>
+      </c>
+      <c r="F245">
+        <v>39.6</v>
+      </c>
+      <c r="G245">
+        <f t="shared" si="1"/>
+        <v>13.200000000000003</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>164</v>
+      </c>
+      <c r="B246" t="s">
+        <v>174</v>
+      </c>
+      <c r="C246">
+        <v>134</v>
+      </c>
+      <c r="D246">
+        <v>14</v>
+      </c>
+      <c r="E246">
+        <v>11.2</v>
+      </c>
+      <c r="F246">
+        <v>16.8</v>
+      </c>
+      <c r="G246">
+        <f t="shared" si="1"/>
+        <v>5.6000000000000014</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>164</v>
+      </c>
+      <c r="B247" t="s">
+        <v>175</v>
+      </c>
+      <c r="C247">
+        <v>138</v>
+      </c>
+      <c r="D247">
+        <v>8</v>
+      </c>
+      <c r="E247">
+        <v>6.4</v>
+      </c>
+      <c r="F247">
+        <v>9.6</v>
+      </c>
+      <c r="G247">
+        <f t="shared" si="1"/>
+        <v>3.1999999999999993</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>164</v>
+      </c>
+      <c r="B248" t="s">
+        <v>176</v>
+      </c>
+      <c r="C248">
+        <v>142</v>
+      </c>
+      <c r="D248">
+        <v>5</v>
+      </c>
+      <c r="E248">
+        <v>4</v>
+      </c>
+      <c r="F248">
+        <v>6</v>
+      </c>
+      <c r="G248">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>164</v>
+      </c>
+      <c r="B249" t="s">
+        <v>177</v>
+      </c>
+      <c r="C249">
+        <v>143</v>
+      </c>
+      <c r="D249">
+        <v>21</v>
+      </c>
+      <c r="E249">
+        <v>16.8</v>
+      </c>
+      <c r="F249">
+        <v>25.2</v>
+      </c>
+      <c r="G249">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999986</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>164</v>
+      </c>
+      <c r="B250" t="s">
+        <v>177</v>
+      </c>
+      <c r="C250">
+        <v>143</v>
+      </c>
+      <c r="D250">
+        <v>43</v>
+      </c>
+      <c r="E250">
+        <v>34.4</v>
+      </c>
+      <c r="F250">
+        <v>51.6</v>
+      </c>
+      <c r="G250">
+        <f t="shared" si="1"/>
+        <v>17.200000000000003</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>164</v>
+      </c>
+      <c r="B251" t="s">
+        <v>177</v>
+      </c>
+      <c r="C251">
+        <v>143</v>
+      </c>
+      <c r="D251">
+        <v>77</v>
+      </c>
+      <c r="E251">
+        <v>61.6</v>
+      </c>
+      <c r="F251">
+        <v>92.4</v>
+      </c>
+      <c r="G251">
+        <f t="shared" si="1"/>
+        <v>30.800000000000004</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>164</v>
+      </c>
+      <c r="B252" t="s">
+        <v>178</v>
+      </c>
+      <c r="C252">
+        <v>144</v>
+      </c>
+      <c r="D252">
+        <v>11</v>
+      </c>
+      <c r="E252">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F252">
+        <v>13.2</v>
+      </c>
+      <c r="G252">
+        <f t="shared" si="1"/>
+        <v>4.3999999999999986</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>164</v>
+      </c>
+      <c r="B253" t="s">
+        <v>178</v>
+      </c>
+      <c r="C253">
+        <v>144</v>
+      </c>
+      <c r="D253">
+        <v>55</v>
+      </c>
+      <c r="E253">
+        <v>44</v>
+      </c>
+      <c r="F253">
+        <v>66</v>
+      </c>
+      <c r="G253">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>164</v>
+      </c>
+      <c r="B254" t="s">
+        <v>178</v>
+      </c>
+      <c r="C254">
+        <v>144</v>
+      </c>
+      <c r="D254">
+        <v>93</v>
+      </c>
+      <c r="E254">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="F254">
+        <v>111.6</v>
+      </c>
+      <c r="G254">
+        <f t="shared" si="1"/>
+        <v>37.199999999999989</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>164</v>
+      </c>
+      <c r="B255" t="s">
+        <v>178</v>
+      </c>
+      <c r="C255">
+        <v>144</v>
+      </c>
+      <c r="D255">
+        <v>118</v>
+      </c>
+      <c r="E255">
+        <v>94.4</v>
+      </c>
+      <c r="F255">
+        <v>141.6</v>
+      </c>
+      <c r="G255">
+        <f t="shared" si="1"/>
+        <v>47.199999999999989</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>164</v>
+      </c>
+      <c r="B256" t="s">
+        <v>178</v>
+      </c>
+      <c r="C256">
+        <v>144</v>
+      </c>
+      <c r="D256">
+        <v>164</v>
+      </c>
+      <c r="E256">
+        <v>131.19999999999999</v>
+      </c>
+      <c r="F256">
+        <v>196.8</v>
+      </c>
+      <c r="G256">
+        <f t="shared" si="1"/>
+        <v>65.600000000000023</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>164</v>
+      </c>
+      <c r="B257" t="s">
+        <v>165</v>
+      </c>
+      <c r="C257">
+        <v>145</v>
+      </c>
+      <c r="D257">
+        <v>1</v>
+      </c>
+      <c r="E257">
+        <v>0.8</v>
+      </c>
+      <c r="F257">
+        <v>1.2</v>
+      </c>
+      <c r="G257">
+        <f t="shared" si="1"/>
+        <v>0.39999999999999991</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>164</v>
+      </c>
+      <c r="B258" t="s">
+        <v>165</v>
+      </c>
+      <c r="C258">
+        <v>145</v>
+      </c>
+      <c r="D258">
+        <v>2</v>
+      </c>
+      <c r="E258">
+        <v>1.6</v>
+      </c>
+      <c r="F258">
+        <v>2.4</v>
+      </c>
+      <c r="G258">
+        <f t="shared" si="1"/>
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>164</v>
+      </c>
+      <c r="B259" t="s">
+        <v>165</v>
+      </c>
+      <c r="C259">
+        <v>145</v>
+      </c>
+      <c r="D259">
+        <v>2</v>
+      </c>
+      <c r="E259">
+        <v>1.6</v>
+      </c>
+      <c r="F259">
+        <v>2.4</v>
+      </c>
+      <c r="G259">
+        <f t="shared" si="1"/>
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>164</v>
+      </c>
+      <c r="B260" t="s">
+        <v>165</v>
+      </c>
+      <c r="C260">
+        <v>145</v>
+      </c>
+      <c r="D260">
+        <v>3</v>
+      </c>
+      <c r="E260">
+        <v>2.4</v>
+      </c>
+      <c r="F260">
+        <v>3.6</v>
+      </c>
+      <c r="G260">
+        <f t="shared" si="1"/>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>164</v>
+      </c>
+      <c r="B261" t="s">
+        <v>165</v>
+      </c>
+      <c r="C261">
+        <v>145</v>
+      </c>
+      <c r="D261">
+        <v>4</v>
+      </c>
+      <c r="E261">
+        <v>3.2</v>
+      </c>
+      <c r="F261">
+        <v>4.8</v>
+      </c>
+      <c r="G261">
+        <f t="shared" si="1"/>
+        <v>1.5999999999999996</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>164</v>
+      </c>
+      <c r="B262" t="s">
+        <v>165</v>
+      </c>
+      <c r="C262">
+        <v>145</v>
+      </c>
+      <c r="D262">
+        <v>5</v>
+      </c>
+      <c r="E262">
+        <v>4</v>
+      </c>
+      <c r="F262">
+        <v>6</v>
+      </c>
+      <c r="G262">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>164</v>
+      </c>
+      <c r="B263" t="s">
+        <v>165</v>
+      </c>
+      <c r="C263">
+        <v>145</v>
+      </c>
+      <c r="D263">
+        <v>7</v>
+      </c>
+      <c r="E263">
+        <v>5.6</v>
+      </c>
+      <c r="F263">
+        <v>8.4</v>
+      </c>
+      <c r="G263">
+        <f t="shared" si="1"/>
+        <v>2.8000000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -14774,10 +17772,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2803F26B-B814-704C-B2A0-A5DB14B7449B}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14788,7 +17786,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>161</v>
       </c>
     </row>
@@ -14811,57 +17809,57 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>16.722611000000001</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>-62.551471499999998</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="5">
         <v>45838</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>16.907081399999999</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>-62.973188200000003</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="5">
         <v>45884</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>16.6669147</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>-63.201355999999997</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="5">
         <v>45982</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>162</v>
       </c>
     </row>
@@ -14875,11 +17873,11 @@
       <c r="C7" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>168</v>
+      <c r="D7" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>60</v>
@@ -14887,7 +17885,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B8" s="5">
         <v>45838</v>
@@ -14907,7 +17905,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B9" s="5">
         <v>45843</v>
@@ -14927,7 +17925,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B10" s="5">
         <v>45848</v>
@@ -14947,7 +17945,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B11" s="5">
         <v>45853</v>
@@ -14967,7 +17965,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B12" s="5">
         <v>45860</v>
@@ -14987,7 +17985,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B13" s="5">
         <v>45868</v>
@@ -15007,7 +18005,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B14" s="5">
         <v>45884</v>
@@ -15027,7 +18025,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B15" s="5">
         <v>45896</v>
@@ -15047,7 +18045,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B16" s="5">
         <v>45909</v>
@@ -15065,9 +18063,9 @@
         <v>150.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B17" s="5">
         <v>45924</v>
@@ -15085,9 +18083,9 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B18" s="5">
         <v>45939</v>
@@ -15105,9 +18103,9 @@
         <v>100.8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B19" s="5">
         <v>45954</v>
@@ -15125,9 +18123,9 @@
         <v>145.69999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B20" s="5">
         <v>45969</v>
@@ -15145,9 +18143,9 @@
         <v>117.3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B21" s="5">
         <v>45984</v>
@@ -15165,9 +18163,9 @@
         <v>115.5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B22" s="5">
         <v>45982</v>
@@ -15183,6 +18181,394 @@
       </c>
       <c r="F22" s="2">
         <v>2.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" s="5">
+        <v>45838</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="E25" s="4">
+        <v>5.3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>7.9</v>
+      </c>
+      <c r="G25">
+        <f>F25-E25</f>
+        <v>2.6000000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="5">
+        <v>45843</v>
+      </c>
+      <c r="C26" s="4">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>30.6</v>
+      </c>
+      <c r="E26" s="4">
+        <v>24.5</v>
+      </c>
+      <c r="F26" s="4">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G39" si="0">F26-E26</f>
+        <v>12.200000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B27" s="5">
+        <v>45848</v>
+      </c>
+      <c r="C27" s="4">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2">
+        <v>172.8</v>
+      </c>
+      <c r="E27" s="4">
+        <v>138.19999999999999</v>
+      </c>
+      <c r="F27" s="4">
+        <v>207.4</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>69.200000000000017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" s="5">
+        <v>45853</v>
+      </c>
+      <c r="C28" s="4">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2">
+        <v>117.2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>93.8</v>
+      </c>
+      <c r="F28" s="4">
+        <v>140.6</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>46.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" s="5">
+        <v>45860</v>
+      </c>
+      <c r="C29" s="4">
+        <v>23</v>
+      </c>
+      <c r="D29" s="2">
+        <v>147.19999999999999</v>
+      </c>
+      <c r="E29" s="4">
+        <v>117.8</v>
+      </c>
+      <c r="F29" s="4">
+        <v>176.6</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>58.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" s="5">
+        <v>45868</v>
+      </c>
+      <c r="C30" s="4">
+        <v>31</v>
+      </c>
+      <c r="D30" s="2">
+        <v>126.2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>101</v>
+      </c>
+      <c r="F30" s="4">
+        <v>151.4</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>50.400000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="5">
+        <v>45884</v>
+      </c>
+      <c r="C31" s="4">
+        <v>47</v>
+      </c>
+      <c r="D31" s="2">
+        <v>119.9</v>
+      </c>
+      <c r="E31" s="4">
+        <v>96</v>
+      </c>
+      <c r="F31" s="4">
+        <v>143.9</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>47.900000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B32" s="5">
+        <v>45896</v>
+      </c>
+      <c r="C32" s="4">
+        <v>59</v>
+      </c>
+      <c r="D32" s="2">
+        <v>155.9</v>
+      </c>
+      <c r="E32" s="4">
+        <v>124.7</v>
+      </c>
+      <c r="F32" s="4">
+        <v>187.1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>62.399999999999991</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B33" s="5">
+        <v>45909</v>
+      </c>
+      <c r="C33" s="4">
+        <v>72</v>
+      </c>
+      <c r="D33" s="2">
+        <v>150.5</v>
+      </c>
+      <c r="E33" s="4">
+        <v>120.4</v>
+      </c>
+      <c r="F33" s="4">
+        <v>180.6</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>60.199999999999989</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34" s="5">
+        <v>45924</v>
+      </c>
+      <c r="C34" s="4">
+        <v>87</v>
+      </c>
+      <c r="D34" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E34" s="4">
+        <v>26</v>
+      </c>
+      <c r="F34" s="4">
+        <v>39</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B35" s="5">
+        <v>45939</v>
+      </c>
+      <c r="C35" s="4">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2">
+        <v>100.8</v>
+      </c>
+      <c r="E35" s="4">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="F35" s="4">
+        <v>121</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>40.400000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" s="5">
+        <v>45954</v>
+      </c>
+      <c r="C36" s="4">
+        <v>117</v>
+      </c>
+      <c r="D36" s="2">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="E36" s="4">
+        <v>116.6</v>
+      </c>
+      <c r="F36" s="4">
+        <v>174.8</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>58.200000000000017</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="5">
+        <v>45969</v>
+      </c>
+      <c r="C37" s="4">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2">
+        <v>117.3</v>
+      </c>
+      <c r="E37" s="4">
+        <v>93.8</v>
+      </c>
+      <c r="F37" s="4">
+        <v>140.80000000000001</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>47.000000000000014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B38" s="5">
+        <v>45984</v>
+      </c>
+      <c r="C38" s="4">
+        <v>147</v>
+      </c>
+      <c r="D38" s="2">
+        <v>115.5</v>
+      </c>
+      <c r="E38" s="4">
+        <v>92.4</v>
+      </c>
+      <c r="F38" s="4">
+        <v>138.6</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>46.199999999999989</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B39" s="5">
+        <v>45982</v>
+      </c>
+      <c r="C39" s="4">
+        <v>145</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E39" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="F39" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>